<commit_message>
zmiana nazwy plików data UJ
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02427279-3C08-445F-BF8D-78F52329B05C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5A4368-B0F4-49FD-8064-75F2734619B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11835" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="40">
   <si>
     <t>Te_cal</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>hh_n1_post_az</t>
+  </si>
+  <si>
+    <t>hh_n1_pre_az_test</t>
   </si>
 </sst>
 </file>
@@ -526,15 +529,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC142"/>
+  <dimension ref="A1:AC187"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C144" sqref="C144"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E143" sqref="E143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -11568,6 +11571,636 @@
       </c>
       <c r="AA142">
         <v>14</v>
+      </c>
+    </row>
+    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>39</v>
+      </c>
+      <c r="B143" t="s">
+        <v>28</v>
+      </c>
+      <c r="C143">
+        <v>5</v>
+      </c>
+      <c r="D143" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>39</v>
+      </c>
+      <c r="B144" t="s">
+        <v>28</v>
+      </c>
+      <c r="C144">
+        <v>5</v>
+      </c>
+      <c r="D144" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>39</v>
+      </c>
+      <c r="B145" t="s">
+        <v>28</v>
+      </c>
+      <c r="C145">
+        <v>5</v>
+      </c>
+      <c r="D145" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>39</v>
+      </c>
+      <c r="B146" t="s">
+        <v>28</v>
+      </c>
+      <c r="C146">
+        <v>10</v>
+      </c>
+      <c r="D146" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>39</v>
+      </c>
+      <c r="B147" t="s">
+        <v>28</v>
+      </c>
+      <c r="C147">
+        <v>10</v>
+      </c>
+      <c r="D147" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>39</v>
+      </c>
+      <c r="B148" t="s">
+        <v>28</v>
+      </c>
+      <c r="C148">
+        <v>10</v>
+      </c>
+      <c r="D148" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>39</v>
+      </c>
+      <c r="B149" t="s">
+        <v>28</v>
+      </c>
+      <c r="C149">
+        <v>15</v>
+      </c>
+      <c r="D149" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>39</v>
+      </c>
+      <c r="B150" t="s">
+        <v>28</v>
+      </c>
+      <c r="C150">
+        <v>15</v>
+      </c>
+      <c r="D150" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>39</v>
+      </c>
+      <c r="B151" t="s">
+        <v>28</v>
+      </c>
+      <c r="C151">
+        <v>15</v>
+      </c>
+      <c r="D151" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>39</v>
+      </c>
+      <c r="B152" t="s">
+        <v>28</v>
+      </c>
+      <c r="C152">
+        <v>20</v>
+      </c>
+      <c r="D152" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>39</v>
+      </c>
+      <c r="B153" t="s">
+        <v>28</v>
+      </c>
+      <c r="C153">
+        <v>20</v>
+      </c>
+      <c r="D153" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>39</v>
+      </c>
+      <c r="B154" t="s">
+        <v>28</v>
+      </c>
+      <c r="C154">
+        <v>20</v>
+      </c>
+      <c r="D154" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>39</v>
+      </c>
+      <c r="B155" t="s">
+        <v>28</v>
+      </c>
+      <c r="C155">
+        <v>25</v>
+      </c>
+      <c r="D155" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>39</v>
+      </c>
+      <c r="B156" t="s">
+        <v>28</v>
+      </c>
+      <c r="C156">
+        <v>25</v>
+      </c>
+      <c r="D156" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>39</v>
+      </c>
+      <c r="B157" t="s">
+        <v>28</v>
+      </c>
+      <c r="C157">
+        <v>25</v>
+      </c>
+      <c r="D157" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>39</v>
+      </c>
+      <c r="B158" t="s">
+        <v>33</v>
+      </c>
+      <c r="C158">
+        <v>5</v>
+      </c>
+      <c r="D158" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>39</v>
+      </c>
+      <c r="B159" t="s">
+        <v>33</v>
+      </c>
+      <c r="C159">
+        <v>5</v>
+      </c>
+      <c r="D159" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>39</v>
+      </c>
+      <c r="B160" t="s">
+        <v>33</v>
+      </c>
+      <c r="C160">
+        <v>5</v>
+      </c>
+      <c r="D160" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>39</v>
+      </c>
+      <c r="B161" t="s">
+        <v>33</v>
+      </c>
+      <c r="C161">
+        <v>10</v>
+      </c>
+      <c r="D161" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>39</v>
+      </c>
+      <c r="B162" t="s">
+        <v>33</v>
+      </c>
+      <c r="C162">
+        <v>10</v>
+      </c>
+      <c r="D162" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>39</v>
+      </c>
+      <c r="B163" t="s">
+        <v>33</v>
+      </c>
+      <c r="C163">
+        <v>10</v>
+      </c>
+      <c r="D163" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>39</v>
+      </c>
+      <c r="B164" t="s">
+        <v>33</v>
+      </c>
+      <c r="C164">
+        <v>15</v>
+      </c>
+      <c r="D164" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>39</v>
+      </c>
+      <c r="B165" t="s">
+        <v>33</v>
+      </c>
+      <c r="C165">
+        <v>15</v>
+      </c>
+      <c r="D165" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>39</v>
+      </c>
+      <c r="B166" t="s">
+        <v>33</v>
+      </c>
+      <c r="C166">
+        <v>15</v>
+      </c>
+      <c r="D166" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>39</v>
+      </c>
+      <c r="B167" t="s">
+        <v>33</v>
+      </c>
+      <c r="C167">
+        <v>20</v>
+      </c>
+      <c r="D167" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>39</v>
+      </c>
+      <c r="B168" t="s">
+        <v>33</v>
+      </c>
+      <c r="C168">
+        <v>20</v>
+      </c>
+      <c r="D168" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>39</v>
+      </c>
+      <c r="B169" t="s">
+        <v>33</v>
+      </c>
+      <c r="C169">
+        <v>20</v>
+      </c>
+      <c r="D169" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>39</v>
+      </c>
+      <c r="B170" t="s">
+        <v>33</v>
+      </c>
+      <c r="C170">
+        <v>25</v>
+      </c>
+      <c r="D170" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>39</v>
+      </c>
+      <c r="B171" t="s">
+        <v>33</v>
+      </c>
+      <c r="C171">
+        <v>25</v>
+      </c>
+      <c r="D171" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>39</v>
+      </c>
+      <c r="B172" t="s">
+        <v>33</v>
+      </c>
+      <c r="C172">
+        <v>25</v>
+      </c>
+      <c r="D172" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>39</v>
+      </c>
+      <c r="B173" t="s">
+        <v>34</v>
+      </c>
+      <c r="C173">
+        <v>5</v>
+      </c>
+      <c r="D173" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>39</v>
+      </c>
+      <c r="B174" t="s">
+        <v>34</v>
+      </c>
+      <c r="C174">
+        <v>5</v>
+      </c>
+      <c r="D174" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>39</v>
+      </c>
+      <c r="B175" t="s">
+        <v>34</v>
+      </c>
+      <c r="C175">
+        <v>5</v>
+      </c>
+      <c r="D175" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>39</v>
+      </c>
+      <c r="B176" t="s">
+        <v>34</v>
+      </c>
+      <c r="C176">
+        <v>10</v>
+      </c>
+      <c r="D176" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>39</v>
+      </c>
+      <c r="B177" t="s">
+        <v>34</v>
+      </c>
+      <c r="C177">
+        <v>10</v>
+      </c>
+      <c r="D177" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>39</v>
+      </c>
+      <c r="B178" t="s">
+        <v>34</v>
+      </c>
+      <c r="C178">
+        <v>10</v>
+      </c>
+      <c r="D178" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>39</v>
+      </c>
+      <c r="B179" t="s">
+        <v>34</v>
+      </c>
+      <c r="C179">
+        <v>15</v>
+      </c>
+      <c r="D179" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>39</v>
+      </c>
+      <c r="B180" t="s">
+        <v>34</v>
+      </c>
+      <c r="C180">
+        <v>15</v>
+      </c>
+      <c r="D180" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>39</v>
+      </c>
+      <c r="B181" t="s">
+        <v>34</v>
+      </c>
+      <c r="C181">
+        <v>15</v>
+      </c>
+      <c r="D181" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>39</v>
+      </c>
+      <c r="B182" t="s">
+        <v>34</v>
+      </c>
+      <c r="C182">
+        <v>20</v>
+      </c>
+      <c r="D182" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>39</v>
+      </c>
+      <c r="B183" t="s">
+        <v>34</v>
+      </c>
+      <c r="C183">
+        <v>20</v>
+      </c>
+      <c r="D183" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>39</v>
+      </c>
+      <c r="B184" t="s">
+        <v>34</v>
+      </c>
+      <c r="C184">
+        <v>20</v>
+      </c>
+      <c r="D184" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>39</v>
+      </c>
+      <c r="B185" t="s">
+        <v>34</v>
+      </c>
+      <c r="C185">
+        <v>25</v>
+      </c>
+      <c r="D185" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>39</v>
+      </c>
+      <c r="B186" t="s">
+        <v>34</v>
+      </c>
+      <c r="C186">
+        <v>25</v>
+      </c>
+      <c r="D186" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>39</v>
+      </c>
+      <c r="B187" t="s">
+        <v>34</v>
+      </c>
+      <c r="C187">
+        <v>25</v>
+      </c>
+      <c r="D187" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
resu_test_7 + close history D1 W1 M1 len5 no atr
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,25 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7943EA3D-4796-4D31-AEDB-9320CB0D6C7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D2EFB5-D634-4815-8B2E-926BD0BFC418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4110" yWindow="870" windowWidth="21600" windowHeight="14625" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$328</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$343</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="47">
   <si>
     <t>Te_cal</t>
   </si>
@@ -173,6 +172,9 @@
   </si>
   <si>
     <t>test6</t>
+  </si>
+  <si>
+    <t>test7</t>
   </si>
 </sst>
 </file>
@@ -548,13 +550,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC343"/>
+  <dimension ref="A1:AC388"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="J308" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E351" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A331" sqref="A331"/>
+      <selection pane="bottomRight" activeCell="E389" sqref="E389"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27126,9 +27128,3462 @@
         <v>10</v>
       </c>
     </row>
+    <row r="344" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A344" t="s">
+        <v>46</v>
+      </c>
+      <c r="B344" t="s">
+        <v>28</v>
+      </c>
+      <c r="C344">
+        <v>5</v>
+      </c>
+      <c r="D344" t="s">
+        <v>26</v>
+      </c>
+      <c r="E344">
+        <v>99.5</v>
+      </c>
+      <c r="F344">
+        <v>60.2</v>
+      </c>
+      <c r="G344">
+        <v>98.5</v>
+      </c>
+      <c r="H344">
+        <v>99.5</v>
+      </c>
+      <c r="I344">
+        <v>99.4</v>
+      </c>
+      <c r="J344">
+        <v>67</v>
+      </c>
+      <c r="K344">
+        <v>23</v>
+      </c>
+      <c r="L344">
+        <v>72.8</v>
+      </c>
+      <c r="M344">
+        <v>10</v>
+      </c>
+      <c r="N344">
+        <v>72.2</v>
+      </c>
+      <c r="O344">
+        <v>14</v>
+      </c>
+      <c r="P344">
+        <v>70.8</v>
+      </c>
+      <c r="Q344">
+        <v>10</v>
+      </c>
+      <c r="R344">
+        <v>69.8</v>
+      </c>
+      <c r="S344">
+        <v>11</v>
+      </c>
+      <c r="T344">
+        <v>58.2</v>
+      </c>
+      <c r="U344">
+        <v>24</v>
+      </c>
+      <c r="V344">
+        <v>61.9</v>
+      </c>
+      <c r="W344">
+        <v>19</v>
+      </c>
+      <c r="X344">
+        <v>62.8</v>
+      </c>
+      <c r="Y344">
+        <v>24</v>
+      </c>
+      <c r="Z344">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="AA344">
+        <v>13</v>
+      </c>
+      <c r="AB344">
+        <v>60.8</v>
+      </c>
+      <c r="AC344">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="345" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A345" t="s">
+        <v>46</v>
+      </c>
+      <c r="B345" t="s">
+        <v>28</v>
+      </c>
+      <c r="C345">
+        <v>5</v>
+      </c>
+      <c r="D345" t="s">
+        <v>29</v>
+      </c>
+      <c r="E345">
+        <v>98.2</v>
+      </c>
+      <c r="F345">
+        <v>60.3</v>
+      </c>
+      <c r="G345">
+        <v>11.4</v>
+      </c>
+      <c r="H345">
+        <v>99.1</v>
+      </c>
+      <c r="I345">
+        <v>97.3</v>
+      </c>
+      <c r="J345">
+        <v>62.3</v>
+      </c>
+      <c r="K345">
+        <v>48</v>
+      </c>
+      <c r="L345">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="M345">
+        <v>21</v>
+      </c>
+      <c r="N345">
+        <v>67.400000000000006</v>
+      </c>
+      <c r="O345">
+        <v>10</v>
+      </c>
+      <c r="T345">
+        <v>61</v>
+      </c>
+      <c r="U345">
+        <v>25</v>
+      </c>
+      <c r="V345">
+        <v>60</v>
+      </c>
+      <c r="W345">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="346" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A346" t="s">
+        <v>46</v>
+      </c>
+      <c r="B346" t="s">
+        <v>28</v>
+      </c>
+      <c r="C346">
+        <v>5</v>
+      </c>
+      <c r="D346" t="s">
+        <v>30</v>
+      </c>
+      <c r="E346">
+        <v>87.4</v>
+      </c>
+      <c r="F346">
+        <v>59.7</v>
+      </c>
+      <c r="G346">
+        <v>100</v>
+      </c>
+      <c r="H346">
+        <v>100</v>
+      </c>
+      <c r="I346">
+        <v>82.3</v>
+      </c>
+      <c r="J346">
+        <v>54.7</v>
+      </c>
+      <c r="K346">
+        <v>83</v>
+      </c>
+      <c r="L346">
+        <v>52.1</v>
+      </c>
+      <c r="M346">
+        <v>100</v>
+      </c>
+      <c r="N346">
+        <v>52.1</v>
+      </c>
+      <c r="O346">
+        <v>100</v>
+      </c>
+      <c r="P346">
+        <v>52.1</v>
+      </c>
+      <c r="Q346">
+        <v>100</v>
+      </c>
+      <c r="R346">
+        <v>52.1</v>
+      </c>
+      <c r="S346">
+        <v>100</v>
+      </c>
+      <c r="T346">
+        <v>61.3</v>
+      </c>
+      <c r="U346">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="347" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A347" t="s">
+        <v>46</v>
+      </c>
+      <c r="B347" t="s">
+        <v>28</v>
+      </c>
+      <c r="C347">
+        <v>10</v>
+      </c>
+      <c r="D347" t="s">
+        <v>26</v>
+      </c>
+      <c r="E347">
+        <v>100</v>
+      </c>
+      <c r="F347">
+        <v>61.9</v>
+      </c>
+      <c r="G347">
+        <v>98.5</v>
+      </c>
+      <c r="H347">
+        <v>100</v>
+      </c>
+      <c r="I347">
+        <v>100</v>
+      </c>
+      <c r="J347">
+        <v>66.3</v>
+      </c>
+      <c r="K347">
+        <v>43</v>
+      </c>
+      <c r="L347">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="M347">
+        <v>21</v>
+      </c>
+      <c r="N347">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="O347">
+        <v>15</v>
+      </c>
+      <c r="P347">
+        <v>68.3</v>
+      </c>
+      <c r="Q347">
+        <v>11</v>
+      </c>
+      <c r="R347">
+        <v>67.8</v>
+      </c>
+      <c r="S347">
+        <v>13</v>
+      </c>
+      <c r="T347">
+        <v>58.6</v>
+      </c>
+      <c r="U347">
+        <v>57</v>
+      </c>
+      <c r="V347">
+        <v>63.9</v>
+      </c>
+      <c r="W347">
+        <v>18</v>
+      </c>
+      <c r="X347">
+        <v>64.3</v>
+      </c>
+      <c r="Y347">
+        <v>12</v>
+      </c>
+      <c r="Z347">
+        <v>63.4</v>
+      </c>
+      <c r="AA347">
+        <v>15</v>
+      </c>
+      <c r="AB347">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="AC347">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="348" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A348" t="s">
+        <v>46</v>
+      </c>
+      <c r="B348" t="s">
+        <v>28</v>
+      </c>
+      <c r="C348">
+        <v>10</v>
+      </c>
+      <c r="D348" t="s">
+        <v>29</v>
+      </c>
+      <c r="E348">
+        <v>99.7</v>
+      </c>
+      <c r="F348">
+        <v>63.2</v>
+      </c>
+      <c r="G348">
+        <v>11.5</v>
+      </c>
+      <c r="H348">
+        <v>99.9</v>
+      </c>
+      <c r="I348">
+        <v>99.5</v>
+      </c>
+      <c r="J348">
+        <v>61.6</v>
+      </c>
+      <c r="K348">
+        <v>66</v>
+      </c>
+      <c r="L348">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="M348">
+        <v>29</v>
+      </c>
+      <c r="N348">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="O348">
+        <v>11</v>
+      </c>
+      <c r="T348">
+        <v>67.7</v>
+      </c>
+      <c r="U348">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="349" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A349" t="s">
+        <v>46</v>
+      </c>
+      <c r="B349" t="s">
+        <v>28</v>
+      </c>
+      <c r="C349">
+        <v>10</v>
+      </c>
+      <c r="D349" t="s">
+        <v>30</v>
+      </c>
+      <c r="E349">
+        <v>98.8</v>
+      </c>
+      <c r="F349">
+        <v>58</v>
+      </c>
+      <c r="G349">
+        <v>100</v>
+      </c>
+      <c r="H349">
+        <v>100</v>
+      </c>
+      <c r="I349">
+        <v>98.3</v>
+      </c>
+      <c r="J349">
+        <v>66.7</v>
+      </c>
+      <c r="K349">
+        <v>26</v>
+      </c>
+      <c r="L349">
+        <v>70.3</v>
+      </c>
+      <c r="M349">
+        <v>14</v>
+      </c>
+      <c r="N349">
+        <v>52.1</v>
+      </c>
+      <c r="O349">
+        <v>100</v>
+      </c>
+      <c r="P349">
+        <v>52.1</v>
+      </c>
+      <c r="Q349">
+        <v>100</v>
+      </c>
+      <c r="R349">
+        <v>52.1</v>
+      </c>
+      <c r="S349">
+        <v>100</v>
+      </c>
+      <c r="T349">
+        <v>68.3</v>
+      </c>
+      <c r="U349">
+        <v>29</v>
+      </c>
+      <c r="V349">
+        <v>62.4</v>
+      </c>
+      <c r="W349">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="350" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A350" t="s">
+        <v>46</v>
+      </c>
+      <c r="B350" t="s">
+        <v>28</v>
+      </c>
+      <c r="C350">
+        <v>15</v>
+      </c>
+      <c r="D350" t="s">
+        <v>26</v>
+      </c>
+      <c r="E350">
+        <v>100</v>
+      </c>
+      <c r="F350">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="G350">
+        <v>99.8</v>
+      </c>
+      <c r="H350">
+        <v>100</v>
+      </c>
+      <c r="I350">
+        <v>100</v>
+      </c>
+      <c r="J350">
+        <v>67.2</v>
+      </c>
+      <c r="K350">
+        <v>37</v>
+      </c>
+      <c r="L350">
+        <v>68.5</v>
+      </c>
+      <c r="M350">
+        <v>30</v>
+      </c>
+      <c r="N350">
+        <v>76.3</v>
+      </c>
+      <c r="O350">
+        <v>15</v>
+      </c>
+      <c r="P350">
+        <v>79.8</v>
+      </c>
+      <c r="Q350">
+        <v>14</v>
+      </c>
+      <c r="R350">
+        <v>76.7</v>
+      </c>
+      <c r="S350">
+        <v>13</v>
+      </c>
+      <c r="T350">
+        <v>71.7</v>
+      </c>
+      <c r="U350">
+        <v>19</v>
+      </c>
+      <c r="V350">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="W350">
+        <v>15</v>
+      </c>
+      <c r="X350">
+        <v>73.8</v>
+      </c>
+      <c r="Y350">
+        <v>11</v>
+      </c>
+      <c r="Z350">
+        <v>75.5</v>
+      </c>
+      <c r="AA350">
+        <v>11</v>
+      </c>
+      <c r="AB350">
+        <v>71</v>
+      </c>
+      <c r="AC350">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="351" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A351" t="s">
+        <v>46</v>
+      </c>
+      <c r="B351" t="s">
+        <v>28</v>
+      </c>
+      <c r="C351">
+        <v>15</v>
+      </c>
+      <c r="D351" t="s">
+        <v>29</v>
+      </c>
+      <c r="E351">
+        <v>100</v>
+      </c>
+      <c r="F351">
+        <v>59</v>
+      </c>
+      <c r="G351">
+        <v>27.2</v>
+      </c>
+      <c r="H351">
+        <v>100</v>
+      </c>
+      <c r="I351">
+        <v>99.9</v>
+      </c>
+      <c r="J351">
+        <v>57.1</v>
+      </c>
+      <c r="K351">
+        <v>77</v>
+      </c>
+      <c r="L351">
+        <v>71</v>
+      </c>
+      <c r="M351">
+        <v>30</v>
+      </c>
+      <c r="N351">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="O351">
+        <v>17</v>
+      </c>
+      <c r="T351">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="U351">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="352" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A352" t="s">
+        <v>46</v>
+      </c>
+      <c r="B352" t="s">
+        <v>28</v>
+      </c>
+      <c r="C352">
+        <v>15</v>
+      </c>
+      <c r="D352" t="s">
+        <v>30</v>
+      </c>
+      <c r="E352">
+        <v>100</v>
+      </c>
+      <c r="F352">
+        <v>64.8</v>
+      </c>
+      <c r="G352">
+        <v>100</v>
+      </c>
+      <c r="H352">
+        <v>100</v>
+      </c>
+      <c r="I352">
+        <v>100</v>
+      </c>
+      <c r="J352">
+        <v>60.3</v>
+      </c>
+      <c r="K352">
+        <v>71</v>
+      </c>
+      <c r="L352">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="M352">
+        <v>12</v>
+      </c>
+      <c r="N352">
+        <v>61.5</v>
+      </c>
+      <c r="O352">
+        <v>41</v>
+      </c>
+      <c r="P352">
+        <v>59.9</v>
+      </c>
+      <c r="Q352">
+        <v>15</v>
+      </c>
+      <c r="T352">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="U352">
+        <v>13</v>
+      </c>
+      <c r="V352">
+        <v>55.4</v>
+      </c>
+      <c r="W352">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="353" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A353" t="s">
+        <v>46</v>
+      </c>
+      <c r="B353" t="s">
+        <v>28</v>
+      </c>
+      <c r="C353">
+        <v>20</v>
+      </c>
+      <c r="D353" t="s">
+        <v>26</v>
+      </c>
+      <c r="E353">
+        <v>100</v>
+      </c>
+      <c r="F353">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="G353">
+        <v>99.8</v>
+      </c>
+      <c r="H353">
+        <v>100</v>
+      </c>
+      <c r="I353">
+        <v>100</v>
+      </c>
+      <c r="J353">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="K353">
+        <v>52</v>
+      </c>
+      <c r="L353">
+        <v>74</v>
+      </c>
+      <c r="M353">
+        <v>34</v>
+      </c>
+      <c r="N353">
+        <v>77.7</v>
+      </c>
+      <c r="O353">
+        <v>21</v>
+      </c>
+      <c r="P353">
+        <v>81.8</v>
+      </c>
+      <c r="Q353">
+        <v>11</v>
+      </c>
+      <c r="R353">
+        <v>87.2</v>
+      </c>
+      <c r="S353">
+        <v>20</v>
+      </c>
+      <c r="T353">
+        <v>73.7</v>
+      </c>
+      <c r="U353">
+        <v>21</v>
+      </c>
+      <c r="V353">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="W353">
+        <v>12</v>
+      </c>
+      <c r="X353">
+        <v>80.5</v>
+      </c>
+      <c r="Y353">
+        <v>14</v>
+      </c>
+      <c r="Z353">
+        <v>74</v>
+      </c>
+      <c r="AA353">
+        <v>11</v>
+      </c>
+      <c r="AB353">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="AC353">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="354" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A354" t="s">
+        <v>46</v>
+      </c>
+      <c r="B354" t="s">
+        <v>28</v>
+      </c>
+      <c r="C354">
+        <v>20</v>
+      </c>
+      <c r="D354" t="s">
+        <v>29</v>
+      </c>
+      <c r="E354">
+        <v>100</v>
+      </c>
+      <c r="F354">
+        <v>62.3</v>
+      </c>
+      <c r="G354">
+        <v>13.6</v>
+      </c>
+      <c r="H354">
+        <v>99.9</v>
+      </c>
+      <c r="I354">
+        <v>100</v>
+      </c>
+      <c r="J354">
+        <v>68.7</v>
+      </c>
+      <c r="K354">
+        <v>35</v>
+      </c>
+      <c r="L354">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="M354">
+        <v>25</v>
+      </c>
+      <c r="N354">
+        <v>75.2</v>
+      </c>
+      <c r="O354">
+        <v>12</v>
+      </c>
+      <c r="T354">
+        <v>68.5</v>
+      </c>
+      <c r="U354">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="355" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A355" t="s">
+        <v>46</v>
+      </c>
+      <c r="B355" t="s">
+        <v>28</v>
+      </c>
+      <c r="C355">
+        <v>20</v>
+      </c>
+      <c r="D355" t="s">
+        <v>30</v>
+      </c>
+      <c r="E355">
+        <v>100</v>
+      </c>
+      <c r="F355">
+        <v>70.5</v>
+      </c>
+      <c r="G355">
+        <v>100</v>
+      </c>
+      <c r="H355">
+        <v>100</v>
+      </c>
+      <c r="I355">
+        <v>100</v>
+      </c>
+      <c r="J355">
+        <v>81.7</v>
+      </c>
+      <c r="K355">
+        <v>11</v>
+      </c>
+      <c r="L355">
+        <v>86.9</v>
+      </c>
+      <c r="M355">
+        <v>19</v>
+      </c>
+      <c r="N355">
+        <v>86.3</v>
+      </c>
+      <c r="O355">
+        <v>10</v>
+      </c>
+      <c r="P355">
+        <v>63.2</v>
+      </c>
+      <c r="Q355">
+        <v>16</v>
+      </c>
+      <c r="R355">
+        <v>52.1</v>
+      </c>
+      <c r="S355">
+        <v>100</v>
+      </c>
+      <c r="T355">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="U355">
+        <v>15</v>
+      </c>
+      <c r="V355">
+        <v>79.8</v>
+      </c>
+      <c r="W355">
+        <v>11</v>
+      </c>
+      <c r="X355">
+        <v>48.4</v>
+      </c>
+      <c r="Y355">
+        <v>99</v>
+      </c>
+      <c r="Z355">
+        <v>52.9</v>
+      </c>
+      <c r="AA355">
+        <v>85</v>
+      </c>
+      <c r="AB355">
+        <v>47.9</v>
+      </c>
+      <c r="AC355">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="356" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A356" t="s">
+        <v>46</v>
+      </c>
+      <c r="B356" t="s">
+        <v>28</v>
+      </c>
+      <c r="C356">
+        <v>25</v>
+      </c>
+      <c r="D356" t="s">
+        <v>26</v>
+      </c>
+      <c r="E356">
+        <v>100</v>
+      </c>
+      <c r="F356">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="G356">
+        <v>99.8</v>
+      </c>
+      <c r="H356">
+        <v>100</v>
+      </c>
+      <c r="I356">
+        <v>100</v>
+      </c>
+      <c r="J356">
+        <v>73.2</v>
+      </c>
+      <c r="K356">
+        <v>31</v>
+      </c>
+      <c r="L356">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M356">
+        <v>21</v>
+      </c>
+      <c r="N356">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="O356">
+        <v>34</v>
+      </c>
+      <c r="P356">
+        <v>82.3</v>
+      </c>
+      <c r="Q356">
+        <v>22</v>
+      </c>
+      <c r="R356">
+        <v>86</v>
+      </c>
+      <c r="S356">
+        <v>11</v>
+      </c>
+      <c r="T356">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="U356">
+        <v>22</v>
+      </c>
+      <c r="V356">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="W356">
+        <v>18</v>
+      </c>
+      <c r="X356">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="Y356">
+        <v>10</v>
+      </c>
+      <c r="Z356">
+        <v>79.5</v>
+      </c>
+      <c r="AA356">
+        <v>23</v>
+      </c>
+      <c r="AB356">
+        <v>77.3</v>
+      </c>
+      <c r="AC356">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="357" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A357" t="s">
+        <v>46</v>
+      </c>
+      <c r="B357" t="s">
+        <v>28</v>
+      </c>
+      <c r="C357">
+        <v>25</v>
+      </c>
+      <c r="D357" t="s">
+        <v>29</v>
+      </c>
+      <c r="E357">
+        <v>100</v>
+      </c>
+      <c r="F357">
+        <v>62.6</v>
+      </c>
+      <c r="G357">
+        <v>13.5</v>
+      </c>
+      <c r="H357">
+        <v>100</v>
+      </c>
+      <c r="I357">
+        <v>100</v>
+      </c>
+      <c r="J357">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="K357">
+        <v>36</v>
+      </c>
+      <c r="L357">
+        <v>72.8</v>
+      </c>
+      <c r="M357">
+        <v>21</v>
+      </c>
+      <c r="N357">
+        <v>73.5</v>
+      </c>
+      <c r="O357">
+        <v>11</v>
+      </c>
+      <c r="T357">
+        <v>67.5</v>
+      </c>
+      <c r="U357">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="358" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A358" t="s">
+        <v>46</v>
+      </c>
+      <c r="B358" t="s">
+        <v>28</v>
+      </c>
+      <c r="C358">
+        <v>25</v>
+      </c>
+      <c r="D358" t="s">
+        <v>30</v>
+      </c>
+      <c r="E358">
+        <v>100</v>
+      </c>
+      <c r="F358">
+        <v>70.8</v>
+      </c>
+      <c r="G358">
+        <v>100</v>
+      </c>
+      <c r="H358">
+        <v>100</v>
+      </c>
+      <c r="I358">
+        <v>100</v>
+      </c>
+      <c r="J358">
+        <v>71</v>
+      </c>
+      <c r="K358">
+        <v>48</v>
+      </c>
+      <c r="L358">
+        <v>84.2</v>
+      </c>
+      <c r="M358">
+        <v>10</v>
+      </c>
+      <c r="N358">
+        <v>84.4</v>
+      </c>
+      <c r="O358">
+        <v>12</v>
+      </c>
+      <c r="P358">
+        <v>52.1</v>
+      </c>
+      <c r="Q358">
+        <v>100</v>
+      </c>
+      <c r="R358">
+        <v>52.1</v>
+      </c>
+      <c r="S358">
+        <v>100</v>
+      </c>
+      <c r="T358">
+        <v>83</v>
+      </c>
+      <c r="U358">
+        <v>11</v>
+      </c>
+      <c r="V358">
+        <v>82.4</v>
+      </c>
+      <c r="W358">
+        <v>12</v>
+      </c>
+      <c r="X358">
+        <v>47.9</v>
+      </c>
+      <c r="Y358">
+        <v>100</v>
+      </c>
+      <c r="Z358">
+        <v>56.7</v>
+      </c>
+      <c r="AA358">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="359" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A359" t="s">
+        <v>46</v>
+      </c>
+      <c r="B359" t="s">
+        <v>33</v>
+      </c>
+      <c r="C359">
+        <v>5</v>
+      </c>
+      <c r="D359" t="s">
+        <v>26</v>
+      </c>
+      <c r="E359">
+        <v>71.8</v>
+      </c>
+      <c r="F359">
+        <v>74.2</v>
+      </c>
+      <c r="G359">
+        <v>43.6</v>
+      </c>
+      <c r="H359">
+        <v>86.6</v>
+      </c>
+      <c r="I359">
+        <v>77.5</v>
+      </c>
+      <c r="J359">
+        <v>77.8</v>
+      </c>
+      <c r="K359">
+        <v>41</v>
+      </c>
+      <c r="L359">
+        <v>86.8</v>
+      </c>
+      <c r="M359">
+        <v>26</v>
+      </c>
+      <c r="N359">
+        <v>90.6</v>
+      </c>
+      <c r="O359">
+        <v>15</v>
+      </c>
+      <c r="P359">
+        <v>94.4</v>
+      </c>
+      <c r="Q359">
+        <v>13</v>
+      </c>
+      <c r="T359">
+        <v>78.2</v>
+      </c>
+      <c r="U359">
+        <v>22</v>
+      </c>
+      <c r="V359">
+        <v>79.400000000000006</v>
+      </c>
+      <c r="W359">
+        <v>19</v>
+      </c>
+      <c r="X359">
+        <v>90.2</v>
+      </c>
+      <c r="Y359">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="360" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A360" t="s">
+        <v>46</v>
+      </c>
+      <c r="B360" t="s">
+        <v>33</v>
+      </c>
+      <c r="C360">
+        <v>5</v>
+      </c>
+      <c r="D360" t="s">
+        <v>29</v>
+      </c>
+      <c r="E360">
+        <v>95.9</v>
+      </c>
+      <c r="F360">
+        <v>75</v>
+      </c>
+      <c r="G360">
+        <v>53.2</v>
+      </c>
+      <c r="H360">
+        <v>96.8</v>
+      </c>
+      <c r="I360">
+        <v>94.8</v>
+      </c>
+      <c r="J360">
+        <v>81.400000000000006</v>
+      </c>
+      <c r="K360">
+        <v>42</v>
+      </c>
+      <c r="L360">
+        <v>84.6</v>
+      </c>
+      <c r="M360">
+        <v>34</v>
+      </c>
+      <c r="N360">
+        <v>88.3</v>
+      </c>
+      <c r="O360">
+        <v>21</v>
+      </c>
+      <c r="P360">
+        <v>88.7</v>
+      </c>
+      <c r="Q360">
+        <v>15</v>
+      </c>
+      <c r="T360">
+        <v>72</v>
+      </c>
+      <c r="U360">
+        <v>52</v>
+      </c>
+      <c r="V360">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="W360">
+        <v>36</v>
+      </c>
+      <c r="X360">
+        <v>91.8</v>
+      </c>
+      <c r="Y360">
+        <v>11</v>
+      </c>
+      <c r="Z360">
+        <v>86</v>
+      </c>
+      <c r="AA360">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="361" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A361" t="s">
+        <v>46</v>
+      </c>
+      <c r="B361" t="s">
+        <v>33</v>
+      </c>
+      <c r="C361">
+        <v>5</v>
+      </c>
+      <c r="D361" t="s">
+        <v>30</v>
+      </c>
+      <c r="E361">
+        <v>69.7</v>
+      </c>
+      <c r="F361">
+        <v>72.5</v>
+      </c>
+      <c r="G361">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="H361">
+        <v>100</v>
+      </c>
+      <c r="I361">
+        <v>72.2</v>
+      </c>
+      <c r="J361">
+        <v>88.3</v>
+      </c>
+      <c r="K361">
+        <v>21</v>
+      </c>
+      <c r="L361">
+        <v>88.8</v>
+      </c>
+      <c r="M361">
+        <v>11</v>
+      </c>
+      <c r="N361">
+        <v>94.1</v>
+      </c>
+      <c r="O361">
+        <v>11</v>
+      </c>
+      <c r="P361">
+        <v>90.8</v>
+      </c>
+      <c r="Q361">
+        <v>11</v>
+      </c>
+      <c r="T361">
+        <v>75.3</v>
+      </c>
+      <c r="U361">
+        <v>21</v>
+      </c>
+      <c r="V361">
+        <v>87.1</v>
+      </c>
+      <c r="W361">
+        <v>14</v>
+      </c>
+      <c r="X361">
+        <v>86.1</v>
+      </c>
+      <c r="Y361">
+        <v>13</v>
+      </c>
+      <c r="Z361">
+        <v>81.8</v>
+      </c>
+      <c r="AA361">
+        <v>11</v>
+      </c>
+      <c r="AB361">
+        <v>82.6</v>
+      </c>
+      <c r="AC361">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="362" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A362" t="s">
+        <v>46</v>
+      </c>
+      <c r="B362" t="s">
+        <v>33</v>
+      </c>
+      <c r="C362">
+        <v>10</v>
+      </c>
+      <c r="D362" t="s">
+        <v>26</v>
+      </c>
+      <c r="E362">
+        <v>98.2</v>
+      </c>
+      <c r="F362">
+        <v>72.5</v>
+      </c>
+      <c r="G362">
+        <v>91</v>
+      </c>
+      <c r="H362">
+        <v>98.5</v>
+      </c>
+      <c r="I362">
+        <v>97.9</v>
+      </c>
+      <c r="J362">
+        <v>82</v>
+      </c>
+      <c r="K362">
+        <v>28</v>
+      </c>
+      <c r="L362">
+        <v>90.5</v>
+      </c>
+      <c r="M362">
+        <v>15</v>
+      </c>
+      <c r="N362">
+        <v>88.7</v>
+      </c>
+      <c r="O362">
+        <v>19</v>
+      </c>
+      <c r="P362">
+        <v>91.4</v>
+      </c>
+      <c r="Q362">
+        <v>16</v>
+      </c>
+      <c r="R362">
+        <v>92.3</v>
+      </c>
+      <c r="S362">
+        <v>10</v>
+      </c>
+      <c r="T362">
+        <v>71</v>
+      </c>
+      <c r="U362">
+        <v>39</v>
+      </c>
+      <c r="V362">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="W362">
+        <v>13</v>
+      </c>
+      <c r="X362">
+        <v>85.2</v>
+      </c>
+      <c r="Y362">
+        <v>10</v>
+      </c>
+      <c r="Z362">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="AA362">
+        <v>11</v>
+      </c>
+      <c r="AB362">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="AC362">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="363" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A363" t="s">
+        <v>46</v>
+      </c>
+      <c r="B363" t="s">
+        <v>33</v>
+      </c>
+      <c r="C363">
+        <v>10</v>
+      </c>
+      <c r="D363" t="s">
+        <v>29</v>
+      </c>
+      <c r="E363">
+        <v>98.8</v>
+      </c>
+      <c r="F363">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G363">
+        <v>50.2</v>
+      </c>
+      <c r="H363">
+        <v>99.8</v>
+      </c>
+      <c r="I363">
+        <v>97.6</v>
+      </c>
+      <c r="J363">
+        <v>83.4</v>
+      </c>
+      <c r="K363">
+        <v>36</v>
+      </c>
+      <c r="L363">
+        <v>84.8</v>
+      </c>
+      <c r="M363">
+        <v>34</v>
+      </c>
+      <c r="N363">
+        <v>88.5</v>
+      </c>
+      <c r="O363">
+        <v>26</v>
+      </c>
+      <c r="P363">
+        <v>89.2</v>
+      </c>
+      <c r="Q363">
+        <v>19</v>
+      </c>
+      <c r="T363">
+        <v>70.3</v>
+      </c>
+      <c r="U363">
+        <v>51</v>
+      </c>
+      <c r="V363">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="W363">
+        <v>34</v>
+      </c>
+      <c r="X363">
+        <v>78</v>
+      </c>
+      <c r="Y363">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="364" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A364" t="s">
+        <v>46</v>
+      </c>
+      <c r="B364" t="s">
+        <v>33</v>
+      </c>
+      <c r="C364">
+        <v>10</v>
+      </c>
+      <c r="D364" t="s">
+        <v>30</v>
+      </c>
+      <c r="E364">
+        <v>85.9</v>
+      </c>
+      <c r="F364">
+        <v>71.8</v>
+      </c>
+      <c r="G364">
+        <v>49.1</v>
+      </c>
+      <c r="H364">
+        <v>100</v>
+      </c>
+      <c r="I364">
+        <v>85.5</v>
+      </c>
+      <c r="J364">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="K364">
+        <v>46</v>
+      </c>
+      <c r="L364">
+        <v>84.6</v>
+      </c>
+      <c r="M364">
+        <v>13</v>
+      </c>
+      <c r="N364">
+        <v>93.5</v>
+      </c>
+      <c r="O364">
+        <v>10</v>
+      </c>
+      <c r="P364">
+        <v>93.5</v>
+      </c>
+      <c r="Q364">
+        <v>12</v>
+      </c>
+      <c r="T364">
+        <v>69.5</v>
+      </c>
+      <c r="U364">
+        <v>43</v>
+      </c>
+      <c r="V364">
+        <v>77.7</v>
+      </c>
+      <c r="W364">
+        <v>13</v>
+      </c>
+      <c r="X364">
+        <v>83.2</v>
+      </c>
+      <c r="Y364">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="365" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A365" t="s">
+        <v>46</v>
+      </c>
+      <c r="B365" t="s">
+        <v>33</v>
+      </c>
+      <c r="C365">
+        <v>15</v>
+      </c>
+      <c r="D365" t="s">
+        <v>26</v>
+      </c>
+      <c r="E365">
+        <v>98.4</v>
+      </c>
+      <c r="F365">
+        <v>74.7</v>
+      </c>
+      <c r="G365">
+        <v>92.2</v>
+      </c>
+      <c r="H365">
+        <v>98.7</v>
+      </c>
+      <c r="I365">
+        <v>98</v>
+      </c>
+      <c r="J365">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="K365">
+        <v>47</v>
+      </c>
+      <c r="L365">
+        <v>82.8</v>
+      </c>
+      <c r="M365">
+        <v>35</v>
+      </c>
+      <c r="N365">
+        <v>89.5</v>
+      </c>
+      <c r="O365">
+        <v>25</v>
+      </c>
+      <c r="P365">
+        <v>92.5</v>
+      </c>
+      <c r="Q365">
+        <v>20</v>
+      </c>
+      <c r="R365">
+        <v>95.7</v>
+      </c>
+      <c r="S365">
+        <v>10</v>
+      </c>
+      <c r="T365">
+        <v>72.8</v>
+      </c>
+      <c r="U365">
+        <v>48</v>
+      </c>
+      <c r="V365">
+        <v>77.2</v>
+      </c>
+      <c r="W365">
+        <v>36</v>
+      </c>
+      <c r="X365">
+        <v>83.3</v>
+      </c>
+      <c r="Y365">
+        <v>14</v>
+      </c>
+      <c r="Z365">
+        <v>86.1</v>
+      </c>
+      <c r="AA365">
+        <v>12</v>
+      </c>
+      <c r="AB365">
+        <v>80.2</v>
+      </c>
+      <c r="AC365">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="366" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A366" t="s">
+        <v>46</v>
+      </c>
+      <c r="B366" t="s">
+        <v>33</v>
+      </c>
+      <c r="C366">
+        <v>15</v>
+      </c>
+      <c r="D366" t="s">
+        <v>29</v>
+      </c>
+      <c r="E366">
+        <v>99.4</v>
+      </c>
+      <c r="F366">
+        <v>73.5</v>
+      </c>
+      <c r="G366">
+        <v>50.5</v>
+      </c>
+      <c r="H366">
+        <v>99.9</v>
+      </c>
+      <c r="I366">
+        <v>98.8</v>
+      </c>
+      <c r="J366">
+        <v>82.4</v>
+      </c>
+      <c r="K366">
+        <v>37</v>
+      </c>
+      <c r="L366">
+        <v>85.2</v>
+      </c>
+      <c r="M366">
+        <v>34</v>
+      </c>
+      <c r="N366">
+        <v>89</v>
+      </c>
+      <c r="O366">
+        <v>29</v>
+      </c>
+      <c r="P366">
+        <v>89.3</v>
+      </c>
+      <c r="Q366">
+        <v>20</v>
+      </c>
+      <c r="R366">
+        <v>92.3</v>
+      </c>
+      <c r="S366">
+        <v>10</v>
+      </c>
+      <c r="T366">
+        <v>70.2</v>
+      </c>
+      <c r="U366">
+        <v>52</v>
+      </c>
+      <c r="V366">
+        <v>77.2</v>
+      </c>
+      <c r="W366">
+        <v>35</v>
+      </c>
+      <c r="X366">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="Y366">
+        <v>10</v>
+      </c>
+      <c r="Z366">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="AA366">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="367" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A367" t="s">
+        <v>46</v>
+      </c>
+      <c r="B367" t="s">
+        <v>33</v>
+      </c>
+      <c r="C367">
+        <v>15</v>
+      </c>
+      <c r="D367" t="s">
+        <v>30</v>
+      </c>
+      <c r="E367">
+        <v>97.9</v>
+      </c>
+      <c r="F367">
+        <v>75</v>
+      </c>
+      <c r="G367">
+        <v>52.6</v>
+      </c>
+      <c r="H367">
+        <v>100</v>
+      </c>
+      <c r="I367">
+        <v>97.6</v>
+      </c>
+      <c r="J367">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="K367">
+        <v>46</v>
+      </c>
+      <c r="L367">
+        <v>84.8</v>
+      </c>
+      <c r="M367">
+        <v>18</v>
+      </c>
+      <c r="N367">
+        <v>94.6</v>
+      </c>
+      <c r="O367">
+        <v>10</v>
+      </c>
+      <c r="P367">
+        <v>93.1</v>
+      </c>
+      <c r="Q367">
+        <v>16</v>
+      </c>
+      <c r="T367">
+        <v>74.5</v>
+      </c>
+      <c r="U367">
+        <v>18</v>
+      </c>
+      <c r="V367">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="W367">
+        <v>26</v>
+      </c>
+      <c r="X367">
+        <v>86.3</v>
+      </c>
+      <c r="Y367">
+        <v>13</v>
+      </c>
+      <c r="Z367">
+        <v>77.3</v>
+      </c>
+      <c r="AA367">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="368" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A368" t="s">
+        <v>46</v>
+      </c>
+      <c r="B368" t="s">
+        <v>33</v>
+      </c>
+      <c r="C368">
+        <v>20</v>
+      </c>
+      <c r="D368" t="s">
+        <v>26</v>
+      </c>
+      <c r="E368">
+        <v>99.4</v>
+      </c>
+      <c r="F368">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="G368">
+        <v>92.4</v>
+      </c>
+      <c r="H368">
+        <v>99.5</v>
+      </c>
+      <c r="I368">
+        <v>99.2</v>
+      </c>
+      <c r="J368">
+        <v>78.7</v>
+      </c>
+      <c r="K368">
+        <v>46</v>
+      </c>
+      <c r="L368">
+        <v>83</v>
+      </c>
+      <c r="M368">
+        <v>35</v>
+      </c>
+      <c r="N368">
+        <v>89</v>
+      </c>
+      <c r="O368">
+        <v>25</v>
+      </c>
+      <c r="P368">
+        <v>93.5</v>
+      </c>
+      <c r="Q368">
+        <v>15</v>
+      </c>
+      <c r="R368">
+        <v>96.8</v>
+      </c>
+      <c r="S368">
+        <v>10</v>
+      </c>
+      <c r="T368">
+        <v>73.8</v>
+      </c>
+      <c r="U368">
+        <v>24</v>
+      </c>
+      <c r="V368">
+        <v>78.3</v>
+      </c>
+      <c r="W368">
+        <v>14</v>
+      </c>
+      <c r="X368">
+        <v>85.8</v>
+      </c>
+      <c r="Y368">
+        <v>14</v>
+      </c>
+      <c r="Z368">
+        <v>85.7</v>
+      </c>
+      <c r="AA368">
+        <v>11</v>
+      </c>
+      <c r="AB368">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="AC368">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="369" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A369" t="s">
+        <v>46</v>
+      </c>
+      <c r="B369" t="s">
+        <v>33</v>
+      </c>
+      <c r="C369">
+        <v>20</v>
+      </c>
+      <c r="D369" t="s">
+        <v>29</v>
+      </c>
+      <c r="E369">
+        <v>99.7</v>
+      </c>
+      <c r="F369">
+        <v>73.8</v>
+      </c>
+      <c r="G369">
+        <v>51.1</v>
+      </c>
+      <c r="H369">
+        <v>100</v>
+      </c>
+      <c r="I369">
+        <v>99.4</v>
+      </c>
+      <c r="J369">
+        <v>82.4</v>
+      </c>
+      <c r="K369">
+        <v>36</v>
+      </c>
+      <c r="L369">
+        <v>84.9</v>
+      </c>
+      <c r="M369">
+        <v>34</v>
+      </c>
+      <c r="N369">
+        <v>89.5</v>
+      </c>
+      <c r="O369">
+        <v>27</v>
+      </c>
+      <c r="P369">
+        <v>91.6</v>
+      </c>
+      <c r="Q369">
+        <v>19</v>
+      </c>
+      <c r="R369">
+        <v>96.6</v>
+      </c>
+      <c r="S369">
+        <v>10</v>
+      </c>
+      <c r="T369">
+        <v>70.900000000000006</v>
+      </c>
+      <c r="U369">
+        <v>52</v>
+      </c>
+      <c r="V369">
+        <v>77.2</v>
+      </c>
+      <c r="W369">
+        <v>35</v>
+      </c>
+      <c r="X369">
+        <v>79.7</v>
+      </c>
+      <c r="Y369">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="370" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A370" t="s">
+        <v>46</v>
+      </c>
+      <c r="B370" t="s">
+        <v>33</v>
+      </c>
+      <c r="C370">
+        <v>20</v>
+      </c>
+      <c r="D370" t="s">
+        <v>30</v>
+      </c>
+      <c r="E370">
+        <v>99.9</v>
+      </c>
+      <c r="F370">
+        <v>74</v>
+      </c>
+      <c r="G370">
+        <v>49.4</v>
+      </c>
+      <c r="H370">
+        <v>100</v>
+      </c>
+      <c r="I370">
+        <v>99.9</v>
+      </c>
+      <c r="J370">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="K370">
+        <v>46</v>
+      </c>
+      <c r="L370">
+        <v>84.4</v>
+      </c>
+      <c r="M370">
+        <v>35</v>
+      </c>
+      <c r="N370">
+        <v>92.6</v>
+      </c>
+      <c r="O370">
+        <v>10</v>
+      </c>
+      <c r="P370">
+        <v>93.8</v>
+      </c>
+      <c r="Q370">
+        <v>12</v>
+      </c>
+      <c r="T370">
+        <v>73</v>
+      </c>
+      <c r="U370">
+        <v>22</v>
+      </c>
+      <c r="V370">
+        <v>78.7</v>
+      </c>
+      <c r="W370">
+        <v>29</v>
+      </c>
+      <c r="X370">
+        <v>87.9</v>
+      </c>
+      <c r="Y370">
+        <v>14</v>
+      </c>
+      <c r="Z370">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="AA370">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="371" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A371" t="s">
+        <v>46</v>
+      </c>
+      <c r="B371" t="s">
+        <v>33</v>
+      </c>
+      <c r="C371">
+        <v>25</v>
+      </c>
+      <c r="D371" t="s">
+        <v>26</v>
+      </c>
+      <c r="E371">
+        <v>100</v>
+      </c>
+      <c r="F371">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G371">
+        <v>94.7</v>
+      </c>
+      <c r="H371">
+        <v>99.9</v>
+      </c>
+      <c r="I371">
+        <v>100</v>
+      </c>
+      <c r="J371">
+        <v>76.7</v>
+      </c>
+      <c r="K371">
+        <v>44</v>
+      </c>
+      <c r="L371">
+        <v>82.8</v>
+      </c>
+      <c r="M371">
+        <v>39</v>
+      </c>
+      <c r="N371">
+        <v>86.4</v>
+      </c>
+      <c r="O371">
+        <v>28</v>
+      </c>
+      <c r="P371">
+        <v>93.5</v>
+      </c>
+      <c r="Q371">
+        <v>17</v>
+      </c>
+      <c r="R371">
+        <v>96</v>
+      </c>
+      <c r="S371">
+        <v>11</v>
+      </c>
+      <c r="T371">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="U371">
+        <v>36</v>
+      </c>
+      <c r="V371">
+        <v>80.400000000000006</v>
+      </c>
+      <c r="W371">
+        <v>29</v>
+      </c>
+      <c r="X371">
+        <v>86.6</v>
+      </c>
+      <c r="Y371">
+        <v>13</v>
+      </c>
+      <c r="Z371">
+        <v>84.5</v>
+      </c>
+      <c r="AA371">
+        <v>11</v>
+      </c>
+      <c r="AB371">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="AC371">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="372" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A372" t="s">
+        <v>46</v>
+      </c>
+      <c r="B372" t="s">
+        <v>33</v>
+      </c>
+      <c r="C372">
+        <v>25</v>
+      </c>
+      <c r="D372" t="s">
+        <v>29</v>
+      </c>
+      <c r="E372">
+        <v>99.9</v>
+      </c>
+      <c r="F372">
+        <v>73.5</v>
+      </c>
+      <c r="G372">
+        <v>43.7</v>
+      </c>
+      <c r="H372">
+        <v>100</v>
+      </c>
+      <c r="I372">
+        <v>99.8</v>
+      </c>
+      <c r="J372">
+        <v>82.4</v>
+      </c>
+      <c r="K372">
+        <v>36</v>
+      </c>
+      <c r="L372">
+        <v>85.4</v>
+      </c>
+      <c r="M372">
+        <v>34</v>
+      </c>
+      <c r="N372">
+        <v>88.6</v>
+      </c>
+      <c r="O372">
+        <v>27</v>
+      </c>
+      <c r="P372">
+        <v>91.3</v>
+      </c>
+      <c r="Q372">
+        <v>16</v>
+      </c>
+      <c r="T372">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="U372">
+        <v>52</v>
+      </c>
+      <c r="V372">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="W372">
+        <v>36</v>
+      </c>
+      <c r="X372">
+        <v>82.4</v>
+      </c>
+      <c r="Y372">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="373" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A373" t="s">
+        <v>46</v>
+      </c>
+      <c r="B373" t="s">
+        <v>33</v>
+      </c>
+      <c r="C373">
+        <v>25</v>
+      </c>
+      <c r="D373" t="s">
+        <v>30</v>
+      </c>
+      <c r="E373">
+        <v>100</v>
+      </c>
+      <c r="F373">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="G373">
+        <v>43.3</v>
+      </c>
+      <c r="H373">
+        <v>100</v>
+      </c>
+      <c r="I373">
+        <v>100</v>
+      </c>
+      <c r="J373">
+        <v>77.7</v>
+      </c>
+      <c r="K373">
+        <v>46</v>
+      </c>
+      <c r="L373">
+        <v>89.6</v>
+      </c>
+      <c r="M373">
+        <v>11</v>
+      </c>
+      <c r="N373">
+        <v>92.5</v>
+      </c>
+      <c r="O373">
+        <v>14</v>
+      </c>
+      <c r="P373">
+        <v>94.4</v>
+      </c>
+      <c r="Q373">
+        <v>14</v>
+      </c>
+      <c r="T373">
+        <v>73.599999999999994</v>
+      </c>
+      <c r="U373">
+        <v>47</v>
+      </c>
+      <c r="V373">
+        <v>81</v>
+      </c>
+      <c r="W373">
+        <v>26</v>
+      </c>
+      <c r="X373">
+        <v>87.9</v>
+      </c>
+      <c r="Y373">
+        <v>11</v>
+      </c>
+      <c r="Z373">
+        <v>81.2</v>
+      </c>
+      <c r="AA373">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="374" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A374" t="s">
+        <v>46</v>
+      </c>
+      <c r="B374" t="s">
+        <v>34</v>
+      </c>
+      <c r="C374">
+        <v>5</v>
+      </c>
+      <c r="D374" t="s">
+        <v>26</v>
+      </c>
+      <c r="E374">
+        <v>70.7</v>
+      </c>
+      <c r="F374">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="G374">
+        <v>45.8</v>
+      </c>
+      <c r="H374">
+        <v>88.3</v>
+      </c>
+      <c r="I374">
+        <v>88.4</v>
+      </c>
+      <c r="J374">
+        <v>86.5</v>
+      </c>
+      <c r="K374">
+        <v>27</v>
+      </c>
+      <c r="L374">
+        <v>88.1</v>
+      </c>
+      <c r="M374">
+        <v>24</v>
+      </c>
+      <c r="N374">
+        <v>91.3</v>
+      </c>
+      <c r="O374">
+        <v>11</v>
+      </c>
+      <c r="P374">
+        <v>92.4</v>
+      </c>
+      <c r="Q374">
+        <v>13</v>
+      </c>
+      <c r="T374">
+        <v>79.7</v>
+      </c>
+      <c r="U374">
+        <v>20</v>
+      </c>
+      <c r="V374">
+        <v>81.8</v>
+      </c>
+      <c r="W374">
+        <v>10</v>
+      </c>
+      <c r="X374">
+        <v>84.7</v>
+      </c>
+      <c r="Y374">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="375" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A375" t="s">
+        <v>46</v>
+      </c>
+      <c r="B375" t="s">
+        <v>34</v>
+      </c>
+      <c r="C375">
+        <v>5</v>
+      </c>
+      <c r="D375" t="s">
+        <v>29</v>
+      </c>
+      <c r="E375">
+        <v>96</v>
+      </c>
+      <c r="F375">
+        <v>71.8</v>
+      </c>
+      <c r="G375">
+        <v>55.1</v>
+      </c>
+      <c r="H375">
+        <v>97.6</v>
+      </c>
+      <c r="I375">
+        <v>94.4</v>
+      </c>
+      <c r="J375">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="K375">
+        <v>41</v>
+      </c>
+      <c r="L375">
+        <v>83.9</v>
+      </c>
+      <c r="M375">
+        <v>32</v>
+      </c>
+      <c r="N375">
+        <v>88.2</v>
+      </c>
+      <c r="O375">
+        <v>26</v>
+      </c>
+      <c r="P375">
+        <v>89</v>
+      </c>
+      <c r="Q375">
+        <v>17</v>
+      </c>
+      <c r="T375">
+        <v>68</v>
+      </c>
+      <c r="U375">
+        <v>50</v>
+      </c>
+      <c r="V375">
+        <v>73.3</v>
+      </c>
+      <c r="W375">
+        <v>37</v>
+      </c>
+      <c r="X375">
+        <v>82</v>
+      </c>
+      <c r="Y375">
+        <v>10</v>
+      </c>
+      <c r="Z375">
+        <v>77.2</v>
+      </c>
+      <c r="AA375">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="376" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A376" t="s">
+        <v>46</v>
+      </c>
+      <c r="B376" t="s">
+        <v>34</v>
+      </c>
+      <c r="C376">
+        <v>5</v>
+      </c>
+      <c r="D376" t="s">
+        <v>30</v>
+      </c>
+      <c r="E376">
+        <v>69</v>
+      </c>
+      <c r="F376">
+        <v>72.3</v>
+      </c>
+      <c r="G376">
+        <v>88.5</v>
+      </c>
+      <c r="H376">
+        <v>100</v>
+      </c>
+      <c r="I376">
+        <v>80.8</v>
+      </c>
+      <c r="J376">
+        <v>86.7</v>
+      </c>
+      <c r="K376">
+        <v>26</v>
+      </c>
+      <c r="L376">
+        <v>88.9</v>
+      </c>
+      <c r="M376">
+        <v>15</v>
+      </c>
+      <c r="N376">
+        <v>91.5</v>
+      </c>
+      <c r="O376">
+        <v>13</v>
+      </c>
+      <c r="P376">
+        <v>91</v>
+      </c>
+      <c r="Q376">
+        <v>11</v>
+      </c>
+      <c r="T376">
+        <v>74.7</v>
+      </c>
+      <c r="U376">
+        <v>30</v>
+      </c>
+      <c r="V376">
+        <v>80.3</v>
+      </c>
+      <c r="W376">
+        <v>16</v>
+      </c>
+      <c r="X376">
+        <v>86.5</v>
+      </c>
+      <c r="Y376">
+        <v>10</v>
+      </c>
+      <c r="Z376">
+        <v>82.8</v>
+      </c>
+      <c r="AA376">
+        <v>10</v>
+      </c>
+      <c r="AB376">
+        <v>79.8</v>
+      </c>
+      <c r="AC376">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="377" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A377" t="s">
+        <v>46</v>
+      </c>
+      <c r="B377" t="s">
+        <v>34</v>
+      </c>
+      <c r="C377">
+        <v>10</v>
+      </c>
+      <c r="D377" t="s">
+        <v>26</v>
+      </c>
+      <c r="E377">
+        <v>97.8</v>
+      </c>
+      <c r="F377">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="G377">
+        <v>91.2</v>
+      </c>
+      <c r="H377">
+        <v>97.9</v>
+      </c>
+      <c r="I377">
+        <v>97.7</v>
+      </c>
+      <c r="J377">
+        <v>82</v>
+      </c>
+      <c r="K377">
+        <v>34</v>
+      </c>
+      <c r="L377">
+        <v>90.5</v>
+      </c>
+      <c r="M377">
+        <v>15</v>
+      </c>
+      <c r="N377">
+        <v>89</v>
+      </c>
+      <c r="O377">
+        <v>25</v>
+      </c>
+      <c r="P377">
+        <v>92.8</v>
+      </c>
+      <c r="Q377">
+        <v>16</v>
+      </c>
+      <c r="R377">
+        <v>96.7</v>
+      </c>
+      <c r="S377">
+        <v>10</v>
+      </c>
+      <c r="T377">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="U377">
+        <v>47</v>
+      </c>
+      <c r="V377">
+        <v>77.5</v>
+      </c>
+      <c r="W377">
+        <v>31</v>
+      </c>
+      <c r="X377">
+        <v>85.8</v>
+      </c>
+      <c r="Y377">
+        <v>18</v>
+      </c>
+      <c r="Z377">
+        <v>89.8</v>
+      </c>
+      <c r="AA377">
+        <v>11</v>
+      </c>
+      <c r="AB377">
+        <v>78.099999999999994</v>
+      </c>
+      <c r="AC377">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="378" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A378" t="s">
+        <v>46</v>
+      </c>
+      <c r="B378" t="s">
+        <v>34</v>
+      </c>
+      <c r="C378">
+        <v>10</v>
+      </c>
+      <c r="D378" t="s">
+        <v>29</v>
+      </c>
+      <c r="E378">
+        <v>98.8</v>
+      </c>
+      <c r="F378">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="G378">
+        <v>51</v>
+      </c>
+      <c r="H378">
+        <v>99.9</v>
+      </c>
+      <c r="I378">
+        <v>97.5</v>
+      </c>
+      <c r="J378">
+        <v>80.3</v>
+      </c>
+      <c r="K378">
+        <v>38</v>
+      </c>
+      <c r="L378">
+        <v>84.4</v>
+      </c>
+      <c r="M378">
+        <v>36</v>
+      </c>
+      <c r="N378">
+        <v>88.2</v>
+      </c>
+      <c r="O378">
+        <v>26</v>
+      </c>
+      <c r="P378">
+        <v>90</v>
+      </c>
+      <c r="Q378">
+        <v>14</v>
+      </c>
+      <c r="T378">
+        <v>69.8</v>
+      </c>
+      <c r="U378">
+        <v>51</v>
+      </c>
+      <c r="V378">
+        <v>74.5</v>
+      </c>
+      <c r="W378">
+        <v>39</v>
+      </c>
+      <c r="X378">
+        <v>81</v>
+      </c>
+      <c r="Y378">
+        <v>17</v>
+      </c>
+      <c r="Z378">
+        <v>81.3</v>
+      </c>
+      <c r="AA378">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="379" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A379" t="s">
+        <v>46</v>
+      </c>
+      <c r="B379" t="s">
+        <v>34</v>
+      </c>
+      <c r="C379">
+        <v>10</v>
+      </c>
+      <c r="D379" t="s">
+        <v>30</v>
+      </c>
+      <c r="E379">
+        <v>84.8</v>
+      </c>
+      <c r="F379">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="G379">
+        <v>53</v>
+      </c>
+      <c r="H379">
+        <v>100</v>
+      </c>
+      <c r="I379">
+        <v>83.8</v>
+      </c>
+      <c r="J379">
+        <v>77.5</v>
+      </c>
+      <c r="K379">
+        <v>47</v>
+      </c>
+      <c r="L379">
+        <v>85</v>
+      </c>
+      <c r="M379">
+        <v>16</v>
+      </c>
+      <c r="N379">
+        <v>93.3</v>
+      </c>
+      <c r="O379">
+        <v>10</v>
+      </c>
+      <c r="P379">
+        <v>94.5</v>
+      </c>
+      <c r="Q379">
+        <v>16</v>
+      </c>
+      <c r="T379">
+        <v>72.8</v>
+      </c>
+      <c r="U379">
+        <v>49</v>
+      </c>
+      <c r="V379">
+        <v>79.5</v>
+      </c>
+      <c r="W379">
+        <v>31</v>
+      </c>
+      <c r="X379">
+        <v>87.4</v>
+      </c>
+      <c r="Y379">
+        <v>15</v>
+      </c>
+      <c r="Z379">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="AA379">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="380" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A380" t="s">
+        <v>46</v>
+      </c>
+      <c r="B380" t="s">
+        <v>34</v>
+      </c>
+      <c r="C380">
+        <v>15</v>
+      </c>
+      <c r="D380" t="s">
+        <v>26</v>
+      </c>
+      <c r="E380">
+        <v>85.2</v>
+      </c>
+      <c r="F380">
+        <v>74.8</v>
+      </c>
+      <c r="G380">
+        <v>74.5</v>
+      </c>
+      <c r="H380">
+        <v>86.4</v>
+      </c>
+      <c r="I380">
+        <v>84.7</v>
+      </c>
+      <c r="J380">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="K380">
+        <v>48</v>
+      </c>
+      <c r="L380">
+        <v>82.8</v>
+      </c>
+      <c r="M380">
+        <v>36</v>
+      </c>
+      <c r="N380">
+        <v>88.3</v>
+      </c>
+      <c r="O380">
+        <v>27</v>
+      </c>
+      <c r="P380">
+        <v>94</v>
+      </c>
+      <c r="Q380">
+        <v>13</v>
+      </c>
+      <c r="R380">
+        <v>97.9</v>
+      </c>
+      <c r="S380">
+        <v>10</v>
+      </c>
+      <c r="T380">
+        <v>72.7</v>
+      </c>
+      <c r="U380">
+        <v>47</v>
+      </c>
+      <c r="V380">
+        <v>79.099999999999994</v>
+      </c>
+      <c r="W380">
+        <v>35</v>
+      </c>
+      <c r="X380">
+        <v>88.4</v>
+      </c>
+      <c r="Y380">
+        <v>16</v>
+      </c>
+      <c r="Z380">
+        <v>89.8</v>
+      </c>
+      <c r="AA380">
+        <v>10</v>
+      </c>
+      <c r="AB380">
+        <v>78.7</v>
+      </c>
+      <c r="AC380">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="381" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A381" t="s">
+        <v>46</v>
+      </c>
+      <c r="B381" t="s">
+        <v>34</v>
+      </c>
+      <c r="C381">
+        <v>15</v>
+      </c>
+      <c r="D381" t="s">
+        <v>29</v>
+      </c>
+      <c r="E381">
+        <v>99.3</v>
+      </c>
+      <c r="F381">
+        <v>73.2</v>
+      </c>
+      <c r="G381">
+        <v>48.2</v>
+      </c>
+      <c r="H381">
+        <v>99.9</v>
+      </c>
+      <c r="I381">
+        <v>98.7</v>
+      </c>
+      <c r="J381">
+        <v>80.599999999999994</v>
+      </c>
+      <c r="K381">
+        <v>38</v>
+      </c>
+      <c r="L381">
+        <v>84.5</v>
+      </c>
+      <c r="M381">
+        <v>33</v>
+      </c>
+      <c r="N381">
+        <v>88.3</v>
+      </c>
+      <c r="O381">
+        <v>30</v>
+      </c>
+      <c r="P381">
+        <v>91.6</v>
+      </c>
+      <c r="Q381">
+        <v>19</v>
+      </c>
+      <c r="T381">
+        <v>70.099999999999994</v>
+      </c>
+      <c r="U381">
+        <v>52</v>
+      </c>
+      <c r="V381">
+        <v>75.5</v>
+      </c>
+      <c r="W381">
+        <v>37</v>
+      </c>
+      <c r="X381">
+        <v>81.2</v>
+      </c>
+      <c r="Y381">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="382" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A382" t="s">
+        <v>46</v>
+      </c>
+      <c r="B382" t="s">
+        <v>34</v>
+      </c>
+      <c r="C382">
+        <v>15</v>
+      </c>
+      <c r="D382" t="s">
+        <v>30</v>
+      </c>
+      <c r="E382">
+        <v>98.3</v>
+      </c>
+      <c r="F382">
+        <v>74.7</v>
+      </c>
+      <c r="G382">
+        <v>53.2</v>
+      </c>
+      <c r="H382">
+        <v>100</v>
+      </c>
+      <c r="I382">
+        <v>98.4</v>
+      </c>
+      <c r="J382">
+        <v>78.2</v>
+      </c>
+      <c r="K382">
+        <v>47</v>
+      </c>
+      <c r="L382">
+        <v>87.7</v>
+      </c>
+      <c r="M382">
+        <v>18</v>
+      </c>
+      <c r="N382">
+        <v>94.3</v>
+      </c>
+      <c r="O382">
+        <v>10</v>
+      </c>
+      <c r="P382">
+        <v>94.3</v>
+      </c>
+      <c r="Q382">
+        <v>17</v>
+      </c>
+      <c r="T382">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="U382">
+        <v>45</v>
+      </c>
+      <c r="V382">
+        <v>80.8</v>
+      </c>
+      <c r="W382">
+        <v>28</v>
+      </c>
+      <c r="X382">
+        <v>87.9</v>
+      </c>
+      <c r="Y382">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="383" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A383" t="s">
+        <v>46</v>
+      </c>
+      <c r="B383" t="s">
+        <v>34</v>
+      </c>
+      <c r="C383">
+        <v>20</v>
+      </c>
+      <c r="D383" t="s">
+        <v>26</v>
+      </c>
+      <c r="E383">
+        <v>91.2</v>
+      </c>
+      <c r="F383">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="G383">
+        <v>82</v>
+      </c>
+      <c r="H383">
+        <v>90.1</v>
+      </c>
+      <c r="I383">
+        <v>92.6</v>
+      </c>
+      <c r="J383">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="K383">
+        <v>47</v>
+      </c>
+      <c r="L383">
+        <v>82.3</v>
+      </c>
+      <c r="M383">
+        <v>37</v>
+      </c>
+      <c r="N383">
+        <v>88.8</v>
+      </c>
+      <c r="O383">
+        <v>21</v>
+      </c>
+      <c r="P383">
+        <v>93.5</v>
+      </c>
+      <c r="Q383">
+        <v>17</v>
+      </c>
+      <c r="R383">
+        <v>95.8</v>
+      </c>
+      <c r="S383">
+        <v>10</v>
+      </c>
+      <c r="T383">
+        <v>73.3</v>
+      </c>
+      <c r="U383">
+        <v>45</v>
+      </c>
+      <c r="V383">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="W383">
+        <v>35</v>
+      </c>
+      <c r="X383">
+        <v>84.3</v>
+      </c>
+      <c r="Y383">
+        <v>17</v>
+      </c>
+      <c r="Z383">
+        <v>86.3</v>
+      </c>
+      <c r="AA383">
+        <v>13</v>
+      </c>
+      <c r="AB383">
+        <v>83.3</v>
+      </c>
+      <c r="AC383">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="384" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A384" t="s">
+        <v>46</v>
+      </c>
+      <c r="B384" t="s">
+        <v>34</v>
+      </c>
+      <c r="C384">
+        <v>20</v>
+      </c>
+      <c r="D384" t="s">
+        <v>29</v>
+      </c>
+      <c r="E384">
+        <v>99.6</v>
+      </c>
+      <c r="F384">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="G384">
+        <v>46.1</v>
+      </c>
+      <c r="H384">
+        <v>100</v>
+      </c>
+      <c r="I384">
+        <v>99.1</v>
+      </c>
+      <c r="J384">
+        <v>80.900000000000006</v>
+      </c>
+      <c r="K384">
+        <v>38</v>
+      </c>
+      <c r="L384">
+        <v>85</v>
+      </c>
+      <c r="M384">
+        <v>33</v>
+      </c>
+      <c r="N384">
+        <v>88.5</v>
+      </c>
+      <c r="O384">
+        <v>26</v>
+      </c>
+      <c r="P384">
+        <v>91.3</v>
+      </c>
+      <c r="Q384">
+        <v>19</v>
+      </c>
+      <c r="T384">
+        <v>70.3</v>
+      </c>
+      <c r="U384">
+        <v>51</v>
+      </c>
+      <c r="V384">
+        <v>77.599999999999994</v>
+      </c>
+      <c r="W384">
+        <v>35</v>
+      </c>
+      <c r="X384">
+        <v>85</v>
+      </c>
+      <c r="Y384">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="385" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A385" t="s">
+        <v>46</v>
+      </c>
+      <c r="B385" t="s">
+        <v>34</v>
+      </c>
+      <c r="C385">
+        <v>20</v>
+      </c>
+      <c r="D385" t="s">
+        <v>30</v>
+      </c>
+      <c r="E385">
+        <v>100</v>
+      </c>
+      <c r="F385">
+        <v>74.5</v>
+      </c>
+      <c r="G385">
+        <v>51.7</v>
+      </c>
+      <c r="H385">
+        <v>100</v>
+      </c>
+      <c r="I385">
+        <v>100</v>
+      </c>
+      <c r="J385">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="K385">
+        <v>26</v>
+      </c>
+      <c r="L385">
+        <v>87.2</v>
+      </c>
+      <c r="M385">
+        <v>12</v>
+      </c>
+      <c r="N385">
+        <v>94.6</v>
+      </c>
+      <c r="O385">
+        <v>10</v>
+      </c>
+      <c r="P385">
+        <v>95.2</v>
+      </c>
+      <c r="Q385">
+        <v>11</v>
+      </c>
+      <c r="T385">
+        <v>72.8</v>
+      </c>
+      <c r="U385">
+        <v>45</v>
+      </c>
+      <c r="V385">
+        <v>82.7</v>
+      </c>
+      <c r="W385">
+        <v>21</v>
+      </c>
+      <c r="X385">
+        <v>88</v>
+      </c>
+      <c r="Y385">
+        <v>11</v>
+      </c>
+      <c r="Z385">
+        <v>32.6</v>
+      </c>
+      <c r="AA385">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="386" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A386" t="s">
+        <v>46</v>
+      </c>
+      <c r="B386" t="s">
+        <v>34</v>
+      </c>
+      <c r="C386">
+        <v>25</v>
+      </c>
+      <c r="D386" t="s">
+        <v>26</v>
+      </c>
+      <c r="E386">
+        <v>86.5</v>
+      </c>
+      <c r="F386">
+        <v>74.5</v>
+      </c>
+      <c r="G386">
+        <v>83</v>
+      </c>
+      <c r="H386">
+        <v>87.5</v>
+      </c>
+      <c r="I386">
+        <v>85.3</v>
+      </c>
+      <c r="J386">
+        <v>77.3</v>
+      </c>
+      <c r="K386">
+        <v>49</v>
+      </c>
+      <c r="L386">
+        <v>81.5</v>
+      </c>
+      <c r="M386">
+        <v>38</v>
+      </c>
+      <c r="N386">
+        <v>87.7</v>
+      </c>
+      <c r="O386">
+        <v>25</v>
+      </c>
+      <c r="P386">
+        <v>92.4</v>
+      </c>
+      <c r="Q386">
+        <v>17</v>
+      </c>
+      <c r="R386">
+        <v>97.7</v>
+      </c>
+      <c r="S386">
+        <v>10</v>
+      </c>
+      <c r="T386">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="U386">
+        <v>46</v>
+      </c>
+      <c r="V386">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="W386">
+        <v>35</v>
+      </c>
+      <c r="X386">
+        <v>83.8</v>
+      </c>
+      <c r="Y386">
+        <v>17</v>
+      </c>
+      <c r="Z386">
+        <v>89.8</v>
+      </c>
+      <c r="AA386">
+        <v>10</v>
+      </c>
+      <c r="AB386">
+        <v>82.9</v>
+      </c>
+      <c r="AC386">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="387" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A387" t="s">
+        <v>46</v>
+      </c>
+      <c r="B387" t="s">
+        <v>34</v>
+      </c>
+      <c r="C387">
+        <v>25</v>
+      </c>
+      <c r="D387" t="s">
+        <v>29</v>
+      </c>
+      <c r="E387">
+        <v>99.6</v>
+      </c>
+      <c r="F387">
+        <v>73.2</v>
+      </c>
+      <c r="G387">
+        <v>46.6</v>
+      </c>
+      <c r="H387">
+        <v>100</v>
+      </c>
+      <c r="I387">
+        <v>99.2</v>
+      </c>
+      <c r="J387">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="K387">
+        <v>38</v>
+      </c>
+      <c r="L387">
+        <v>85</v>
+      </c>
+      <c r="M387">
+        <v>33</v>
+      </c>
+      <c r="N387">
+        <v>88.2</v>
+      </c>
+      <c r="O387">
+        <v>27</v>
+      </c>
+      <c r="P387">
+        <v>90.8</v>
+      </c>
+      <c r="Q387">
+        <v>19</v>
+      </c>
+      <c r="T387">
+        <v>69.900000000000006</v>
+      </c>
+      <c r="U387">
+        <v>51</v>
+      </c>
+      <c r="V387">
+        <v>76.5</v>
+      </c>
+      <c r="W387">
+        <v>35</v>
+      </c>
+      <c r="X387">
+        <v>82.9</v>
+      </c>
+      <c r="Y387">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="388" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A388" t="s">
+        <v>46</v>
+      </c>
+      <c r="B388" t="s">
+        <v>34</v>
+      </c>
+      <c r="C388">
+        <v>25</v>
+      </c>
+      <c r="D388" t="s">
+        <v>30</v>
+      </c>
+      <c r="E388">
+        <v>100</v>
+      </c>
+      <c r="F388">
+        <v>73.8</v>
+      </c>
+      <c r="G388">
+        <v>49.5</v>
+      </c>
+      <c r="H388">
+        <v>100</v>
+      </c>
+      <c r="I388">
+        <v>100</v>
+      </c>
+      <c r="J388">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="K388">
+        <v>35</v>
+      </c>
+      <c r="L388">
+        <v>88.9</v>
+      </c>
+      <c r="M388">
+        <v>11</v>
+      </c>
+      <c r="N388">
+        <v>94</v>
+      </c>
+      <c r="O388">
+        <v>11</v>
+      </c>
+      <c r="P388">
+        <v>96</v>
+      </c>
+      <c r="Q388">
+        <v>11</v>
+      </c>
+      <c r="T388">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="U388">
+        <v>16</v>
+      </c>
+      <c r="V388">
+        <v>81.5</v>
+      </c>
+      <c r="W388">
+        <v>26</v>
+      </c>
+      <c r="X388">
+        <v>88.1</v>
+      </c>
+      <c r="Y388">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AC328" xr:uid="{3CACE78E-09B0-4A51-A9AF-2F3B2E4BAEFC}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC313">
+  <autoFilter ref="A1:AC343" xr:uid="{3CACE78E-09B0-4A51-A9AF-2F3B2E4BAEFC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC343">
       <sortCondition ref="A2:A97"/>
       <sortCondition ref="B2:B97"/>
       <sortCondition ref="C2:C97"/>

</xml_diff>

<commit_message>
optymalizacje timeput5min; MLP SVC
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pioo\notebooks\wm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D2EFB5-D634-4815-8B2E-926BD0BFC418}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05B0A514-16C7-4947-A86F-48EEA34FD849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="435" xr2:uid="{B6B0453F-83A4-43EC-A328-DC10FEB5BD2E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1334" uniqueCount="51">
   <si>
     <t>Te_cal</t>
   </si>
@@ -175,6 +175,18 @@
   </si>
   <si>
     <t>test7</t>
+  </si>
+  <si>
+    <t>test8 loc</t>
+  </si>
+  <si>
+    <t>test8 col</t>
+  </si>
+  <si>
+    <t>test 9</t>
+  </si>
+  <si>
+    <t>test10 col</t>
   </si>
 </sst>
 </file>
@@ -550,13 +562,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBA71D6A-A9B1-42AC-9396-7E4A540CDDDA}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AC388"/>
+  <dimension ref="A1:AC436"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E351" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E406" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E389" sqref="E389"/>
+      <selection pane="bottomRight" activeCell="E436" sqref="E436"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30581,9 +30593,1797 @@
         <v>16</v>
       </c>
     </row>
+    <row r="389" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A389" t="s">
+        <v>48</v>
+      </c>
+      <c r="B389" t="s">
+        <v>34</v>
+      </c>
+      <c r="C389">
+        <v>15</v>
+      </c>
+      <c r="D389" t="s">
+        <v>26</v>
+      </c>
+      <c r="E389">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="F389">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="G389">
+        <v>100</v>
+      </c>
+      <c r="H389">
+        <v>100</v>
+      </c>
+      <c r="I389">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="J389">
+        <v>73.3</v>
+      </c>
+      <c r="K389">
+        <v>92</v>
+      </c>
+      <c r="L389">
+        <v>77.099999999999994</v>
+      </c>
+      <c r="M389">
+        <v>74</v>
+      </c>
+      <c r="N389">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="O389">
+        <v>46</v>
+      </c>
+      <c r="P389">
+        <v>87.5</v>
+      </c>
+      <c r="Q389">
+        <v>10</v>
+      </c>
+      <c r="R389">
+        <v>91.5</v>
+      </c>
+      <c r="S389">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="390" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>47</v>
+      </c>
+      <c r="B390" t="s">
+        <v>34</v>
+      </c>
+      <c r="C390">
+        <v>15</v>
+      </c>
+      <c r="D390" t="s">
+        <v>26</v>
+      </c>
+      <c r="E390">
+        <v>73.7</v>
+      </c>
+      <c r="F390">
+        <v>72.2</v>
+      </c>
+      <c r="G390">
+        <v>91.5</v>
+      </c>
+      <c r="H390">
+        <v>100</v>
+      </c>
+      <c r="I390">
+        <v>14.7</v>
+      </c>
+      <c r="J390">
+        <v>72.7</v>
+      </c>
+      <c r="K390">
+        <v>91</v>
+      </c>
+      <c r="L390">
+        <v>76.099999999999994</v>
+      </c>
+      <c r="M390">
+        <v>77</v>
+      </c>
+      <c r="N390">
+        <v>81.099999999999994</v>
+      </c>
+      <c r="O390">
+        <v>49</v>
+      </c>
+      <c r="P390">
+        <v>86.9</v>
+      </c>
+      <c r="Q390">
+        <v>19</v>
+      </c>
+      <c r="R390">
+        <v>90.4</v>
+      </c>
+      <c r="S390">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="391" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>49</v>
+      </c>
+      <c r="B391" t="s">
+        <v>28</v>
+      </c>
+      <c r="C391">
+        <v>5</v>
+      </c>
+      <c r="D391" t="s">
+        <v>26</v>
+      </c>
+      <c r="E391">
+        <v>68</v>
+      </c>
+      <c r="F391">
+        <v>60.5</v>
+      </c>
+      <c r="G391">
+        <v>28.5</v>
+      </c>
+      <c r="H391">
+        <v>100</v>
+      </c>
+      <c r="I391">
+        <v>47.7</v>
+      </c>
+      <c r="T391">
+        <v>44</v>
+      </c>
+      <c r="U391">
+        <v>87</v>
+      </c>
+      <c r="V391">
+        <v>42.6</v>
+      </c>
+      <c r="W391">
+        <v>13</v>
+      </c>
+      <c r="X391">
+        <v>39.6</v>
+      </c>
+      <c r="Y391">
+        <v>12</v>
+      </c>
+      <c r="Z391">
+        <v>35.9</v>
+      </c>
+      <c r="AA391">
+        <v>20</v>
+      </c>
+      <c r="AB391">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AC391">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="392" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>49</v>
+      </c>
+      <c r="B392" t="s">
+        <v>28</v>
+      </c>
+      <c r="C392">
+        <v>5</v>
+      </c>
+      <c r="D392" t="s">
+        <v>29</v>
+      </c>
+      <c r="E392">
+        <v>98.6</v>
+      </c>
+      <c r="F392">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="G392">
+        <v>32.6</v>
+      </c>
+      <c r="H392">
+        <v>99.8</v>
+      </c>
+      <c r="I392">
+        <v>97</v>
+      </c>
+      <c r="T392">
+        <v>43.7</v>
+      </c>
+      <c r="U392">
+        <v>91</v>
+      </c>
+      <c r="V392">
+        <v>41.2</v>
+      </c>
+      <c r="W392">
+        <v>39</v>
+      </c>
+      <c r="X392">
+        <v>31.6</v>
+      </c>
+      <c r="Y392">
+        <v>15</v>
+      </c>
+      <c r="Z392">
+        <v>18.5</v>
+      </c>
+      <c r="AA392">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="393" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>49</v>
+      </c>
+      <c r="B393" t="s">
+        <v>28</v>
+      </c>
+      <c r="C393">
+        <v>5</v>
+      </c>
+      <c r="D393" t="s">
+        <v>30</v>
+      </c>
+      <c r="E393">
+        <v>89</v>
+      </c>
+      <c r="F393">
+        <v>63.7</v>
+      </c>
+      <c r="G393">
+        <v>7.9</v>
+      </c>
+      <c r="H393">
+        <v>100</v>
+      </c>
+      <c r="I393">
+        <v>83.9</v>
+      </c>
+      <c r="T393">
+        <v>43.3</v>
+      </c>
+      <c r="U393">
+        <v>99</v>
+      </c>
+      <c r="V393">
+        <v>43.3</v>
+      </c>
+      <c r="W393">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="394" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>49</v>
+      </c>
+      <c r="B394" t="s">
+        <v>28</v>
+      </c>
+      <c r="C394">
+        <v>10</v>
+      </c>
+      <c r="D394" t="s">
+        <v>26</v>
+      </c>
+      <c r="E394">
+        <v>74.099999999999994</v>
+      </c>
+      <c r="F394">
+        <v>62.3</v>
+      </c>
+      <c r="G394">
+        <v>34.700000000000003</v>
+      </c>
+      <c r="H394">
+        <v>100</v>
+      </c>
+      <c r="I394">
+        <v>61.3</v>
+      </c>
+      <c r="T394">
+        <v>43.9</v>
+      </c>
+      <c r="U394">
+        <v>92</v>
+      </c>
+      <c r="V394">
+        <v>42.7</v>
+      </c>
+      <c r="W394">
+        <v>39</v>
+      </c>
+      <c r="X394">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="Y394">
+        <v>15</v>
+      </c>
+      <c r="Z394">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="AA394">
+        <v>13</v>
+      </c>
+      <c r="AB394">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="AC394">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="395" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>49</v>
+      </c>
+      <c r="B395" t="s">
+        <v>28</v>
+      </c>
+      <c r="C395">
+        <v>10</v>
+      </c>
+      <c r="D395" t="s">
+        <v>29</v>
+      </c>
+      <c r="E395">
+        <v>99.7</v>
+      </c>
+      <c r="F395">
+        <v>68.5</v>
+      </c>
+      <c r="G395">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="H395">
+        <v>100</v>
+      </c>
+      <c r="I395">
+        <v>99.3</v>
+      </c>
+      <c r="T395">
+        <v>43.1</v>
+      </c>
+      <c r="U395">
+        <v>89</v>
+      </c>
+      <c r="V395">
+        <v>40.1</v>
+      </c>
+      <c r="W395">
+        <v>35</v>
+      </c>
+      <c r="X395">
+        <v>33.700000000000003</v>
+      </c>
+      <c r="Y395">
+        <v>10</v>
+      </c>
+      <c r="Z395">
+        <v>19.2</v>
+      </c>
+      <c r="AA395">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="396" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>49</v>
+      </c>
+      <c r="B396" t="s">
+        <v>28</v>
+      </c>
+      <c r="C396">
+        <v>10</v>
+      </c>
+      <c r="D396" t="s">
+        <v>30</v>
+      </c>
+      <c r="E396">
+        <v>100</v>
+      </c>
+      <c r="F396">
+        <v>70.2</v>
+      </c>
+      <c r="G396">
+        <v>25.1</v>
+      </c>
+      <c r="H396">
+        <v>100</v>
+      </c>
+      <c r="I396">
+        <v>100</v>
+      </c>
+      <c r="T396">
+        <v>43.2</v>
+      </c>
+      <c r="U396">
+        <v>100</v>
+      </c>
+      <c r="V396">
+        <v>47.4</v>
+      </c>
+      <c r="W396">
+        <v>15</v>
+      </c>
+      <c r="X396">
+        <v>33</v>
+      </c>
+      <c r="Y396">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="397" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>49</v>
+      </c>
+      <c r="B397" t="s">
+        <v>28</v>
+      </c>
+      <c r="C397">
+        <v>15</v>
+      </c>
+      <c r="D397" t="s">
+        <v>26</v>
+      </c>
+      <c r="E397">
+        <v>78.400000000000006</v>
+      </c>
+      <c r="F397">
+        <v>62.2</v>
+      </c>
+      <c r="G397">
+        <v>40.5</v>
+      </c>
+      <c r="H397">
+        <v>100</v>
+      </c>
+      <c r="I397">
+        <v>65.8</v>
+      </c>
+      <c r="T397">
+        <v>43.7</v>
+      </c>
+      <c r="U397">
+        <v>89</v>
+      </c>
+      <c r="V397">
+        <v>42.4</v>
+      </c>
+      <c r="W397">
+        <v>34</v>
+      </c>
+      <c r="X397">
+        <v>39.4</v>
+      </c>
+      <c r="Y397">
+        <v>25</v>
+      </c>
+      <c r="Z397">
+        <v>38.5</v>
+      </c>
+      <c r="AA397">
+        <v>23</v>
+      </c>
+      <c r="AB397">
+        <v>36</v>
+      </c>
+      <c r="AC397">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="398" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>49</v>
+      </c>
+      <c r="B398" t="s">
+        <v>28</v>
+      </c>
+      <c r="C398">
+        <v>15</v>
+      </c>
+      <c r="D398" t="s">
+        <v>29</v>
+      </c>
+      <c r="E398">
+        <v>100</v>
+      </c>
+      <c r="F398">
+        <v>68.3</v>
+      </c>
+      <c r="G398">
+        <v>28.3</v>
+      </c>
+      <c r="H398">
+        <v>100</v>
+      </c>
+      <c r="I398">
+        <v>100</v>
+      </c>
+      <c r="T398">
+        <v>43.3</v>
+      </c>
+      <c r="U398">
+        <v>89</v>
+      </c>
+      <c r="V398">
+        <v>40.200000000000003</v>
+      </c>
+      <c r="W398">
+        <v>32</v>
+      </c>
+      <c r="X398">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="Y398">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="399" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>49</v>
+      </c>
+      <c r="B399" t="s">
+        <v>28</v>
+      </c>
+      <c r="C399">
+        <v>15</v>
+      </c>
+      <c r="D399" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="400" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>49</v>
+      </c>
+      <c r="B400" t="s">
+        <v>28</v>
+      </c>
+      <c r="C400">
+        <v>20</v>
+      </c>
+      <c r="D400" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="401" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>49</v>
+      </c>
+      <c r="B401" t="s">
+        <v>28</v>
+      </c>
+      <c r="C401">
+        <v>20</v>
+      </c>
+      <c r="D401" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="402" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>49</v>
+      </c>
+      <c r="B402" t="s">
+        <v>28</v>
+      </c>
+      <c r="C402">
+        <v>20</v>
+      </c>
+      <c r="D402" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="403" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>49</v>
+      </c>
+      <c r="B403" t="s">
+        <v>28</v>
+      </c>
+      <c r="C403">
+        <v>25</v>
+      </c>
+      <c r="D403" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="404" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>49</v>
+      </c>
+      <c r="B404" t="s">
+        <v>28</v>
+      </c>
+      <c r="C404">
+        <v>25</v>
+      </c>
+      <c r="D404" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="405" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>49</v>
+      </c>
+      <c r="B405" t="s">
+        <v>28</v>
+      </c>
+      <c r="C405">
+        <v>25</v>
+      </c>
+      <c r="D405" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="406" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>49</v>
+      </c>
+      <c r="B406" t="s">
+        <v>33</v>
+      </c>
+      <c r="C406">
+        <v>5</v>
+      </c>
+      <c r="D406" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="407" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>49</v>
+      </c>
+      <c r="B407" t="s">
+        <v>33</v>
+      </c>
+      <c r="C407">
+        <v>5</v>
+      </c>
+      <c r="D407" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="408" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>49</v>
+      </c>
+      <c r="B408" t="s">
+        <v>33</v>
+      </c>
+      <c r="C408">
+        <v>5</v>
+      </c>
+      <c r="D408" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="409" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>49</v>
+      </c>
+      <c r="B409" t="s">
+        <v>33</v>
+      </c>
+      <c r="C409">
+        <v>10</v>
+      </c>
+      <c r="D409" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="410" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>49</v>
+      </c>
+      <c r="B410" t="s">
+        <v>33</v>
+      </c>
+      <c r="C410">
+        <v>10</v>
+      </c>
+      <c r="D410" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="411" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>49</v>
+      </c>
+      <c r="B411" t="s">
+        <v>33</v>
+      </c>
+      <c r="C411">
+        <v>10</v>
+      </c>
+      <c r="D411" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="412" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>49</v>
+      </c>
+      <c r="B412" t="s">
+        <v>33</v>
+      </c>
+      <c r="C412">
+        <v>15</v>
+      </c>
+      <c r="D412" t="s">
+        <v>26</v>
+      </c>
+      <c r="E412">
+        <v>73.3</v>
+      </c>
+      <c r="F412">
+        <v>62.4</v>
+      </c>
+      <c r="G412">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="H412">
+        <v>100</v>
+      </c>
+      <c r="I412">
+        <v>60.8</v>
+      </c>
+      <c r="T412">
+        <v>43.5</v>
+      </c>
+      <c r="U412">
+        <v>81</v>
+      </c>
+      <c r="V412">
+        <v>41.9</v>
+      </c>
+      <c r="W412">
+        <v>48</v>
+      </c>
+      <c r="X412">
+        <v>41.5</v>
+      </c>
+      <c r="Y412">
+        <v>17</v>
+      </c>
+      <c r="Z412">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="AA412">
+        <v>12</v>
+      </c>
+      <c r="AB412">
+        <v>29.3</v>
+      </c>
+      <c r="AC412">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="413" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>49</v>
+      </c>
+      <c r="B413" t="s">
+        <v>33</v>
+      </c>
+      <c r="C413">
+        <v>15</v>
+      </c>
+      <c r="D413" t="s">
+        <v>29</v>
+      </c>
+      <c r="E413">
+        <v>99.9</v>
+      </c>
+      <c r="F413">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="G413">
+        <v>36.6</v>
+      </c>
+      <c r="H413">
+        <v>100</v>
+      </c>
+      <c r="I413">
+        <v>99.8</v>
+      </c>
+      <c r="T413">
+        <v>41.7</v>
+      </c>
+      <c r="U413">
+        <v>89</v>
+      </c>
+      <c r="V413">
+        <v>39.9</v>
+      </c>
+      <c r="W413">
+        <v>50</v>
+      </c>
+      <c r="X413">
+        <v>24.6</v>
+      </c>
+      <c r="Y413">
+        <v>21</v>
+      </c>
+      <c r="Z413">
+        <v>14.5</v>
+      </c>
+      <c r="AA413">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="414" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>49</v>
+      </c>
+      <c r="B414" t="s">
+        <v>33</v>
+      </c>
+      <c r="C414">
+        <v>15</v>
+      </c>
+      <c r="D414" t="s">
+        <v>30</v>
+      </c>
+      <c r="E414">
+        <v>100</v>
+      </c>
+      <c r="F414">
+        <v>76</v>
+      </c>
+      <c r="G414">
+        <v>44</v>
+      </c>
+      <c r="H414">
+        <v>100</v>
+      </c>
+      <c r="I414">
+        <v>100</v>
+      </c>
+      <c r="T414">
+        <v>44.2</v>
+      </c>
+      <c r="U414">
+        <v>90</v>
+      </c>
+      <c r="V414">
+        <v>44.9</v>
+      </c>
+      <c r="W414">
+        <v>20</v>
+      </c>
+      <c r="X414">
+        <v>28.7</v>
+      </c>
+      <c r="Y414">
+        <v>13</v>
+      </c>
+      <c r="Z414">
+        <v>22</v>
+      </c>
+      <c r="AA414">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="415" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>49</v>
+      </c>
+      <c r="B415" t="s">
+        <v>33</v>
+      </c>
+      <c r="C415">
+        <v>20</v>
+      </c>
+      <c r="D415" t="s">
+        <v>26</v>
+      </c>
+      <c r="E415">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F415">
+        <v>64.8</v>
+      </c>
+      <c r="G415">
+        <v>41</v>
+      </c>
+      <c r="H415">
+        <v>100</v>
+      </c>
+      <c r="I415">
+        <v>63.1</v>
+      </c>
+      <c r="T415">
+        <v>43.3</v>
+      </c>
+      <c r="U415">
+        <v>92</v>
+      </c>
+      <c r="V415">
+        <v>44.5</v>
+      </c>
+      <c r="W415">
+        <v>23</v>
+      </c>
+      <c r="X415">
+        <v>36.5</v>
+      </c>
+      <c r="Y415">
+        <v>16</v>
+      </c>
+      <c r="Z415">
+        <v>29.5</v>
+      </c>
+      <c r="AA415">
+        <v>10</v>
+      </c>
+      <c r="AB415">
+        <v>26.2</v>
+      </c>
+      <c r="AC415">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="416" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>49</v>
+      </c>
+      <c r="B416" t="s">
+        <v>33</v>
+      </c>
+      <c r="C416">
+        <v>20</v>
+      </c>
+      <c r="D416" t="s">
+        <v>29</v>
+      </c>
+      <c r="E416">
+        <v>100</v>
+      </c>
+      <c r="F416">
+        <v>72.8</v>
+      </c>
+      <c r="G416">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="H416">
+        <v>100</v>
+      </c>
+      <c r="I416">
+        <v>99.9</v>
+      </c>
+      <c r="T416">
+        <v>42</v>
+      </c>
+      <c r="U416">
+        <v>90</v>
+      </c>
+      <c r="V416">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="W416">
+        <v>51</v>
+      </c>
+      <c r="X416">
+        <v>24.8</v>
+      </c>
+      <c r="Y416">
+        <v>22</v>
+      </c>
+      <c r="Z416">
+        <v>14.3</v>
+      </c>
+      <c r="AA416">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="417" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>49</v>
+      </c>
+      <c r="B417" t="s">
+        <v>33</v>
+      </c>
+      <c r="C417">
+        <v>20</v>
+      </c>
+      <c r="D417" t="s">
+        <v>30</v>
+      </c>
+      <c r="E417">
+        <v>100</v>
+      </c>
+      <c r="F417">
+        <v>75.099999999999994</v>
+      </c>
+      <c r="G417">
+        <v>43.7</v>
+      </c>
+      <c r="H417">
+        <v>100</v>
+      </c>
+      <c r="I417">
+        <v>100</v>
+      </c>
+      <c r="T417">
+        <v>43.7</v>
+      </c>
+      <c r="U417">
+        <v>88</v>
+      </c>
+      <c r="V417">
+        <v>48.5</v>
+      </c>
+      <c r="W417">
+        <v>14</v>
+      </c>
+      <c r="X417">
+        <v>34.6</v>
+      </c>
+      <c r="Y417">
+        <v>11</v>
+      </c>
+      <c r="Z417">
+        <v>28.9</v>
+      </c>
+      <c r="AA417">
+        <v>10</v>
+      </c>
+      <c r="AB417">
+        <v>18</v>
+      </c>
+      <c r="AC417">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="418" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>49</v>
+      </c>
+      <c r="B418" t="s">
+        <v>33</v>
+      </c>
+      <c r="C418">
+        <v>25</v>
+      </c>
+      <c r="D418" t="s">
+        <v>26</v>
+      </c>
+      <c r="E418">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="F418">
+        <v>66.8</v>
+      </c>
+      <c r="G418">
+        <v>52.7</v>
+      </c>
+      <c r="H418">
+        <v>100</v>
+      </c>
+      <c r="I418">
+        <v>73.8</v>
+      </c>
+      <c r="T418">
+        <v>43.6</v>
+      </c>
+      <c r="U418">
+        <v>82</v>
+      </c>
+      <c r="V418">
+        <v>42.3</v>
+      </c>
+      <c r="W418">
+        <v>46</v>
+      </c>
+      <c r="X418">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="Y418">
+        <v>19</v>
+      </c>
+      <c r="Z418">
+        <v>33.299999999999997</v>
+      </c>
+      <c r="AA418">
+        <v>14</v>
+      </c>
+      <c r="AB418">
+        <v>28.8</v>
+      </c>
+      <c r="AC418">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="419" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>49</v>
+      </c>
+      <c r="B419" t="s">
+        <v>33</v>
+      </c>
+      <c r="C419">
+        <v>25</v>
+      </c>
+      <c r="D419" t="s">
+        <v>29</v>
+      </c>
+      <c r="E419">
+        <v>100</v>
+      </c>
+      <c r="F419">
+        <v>72.8</v>
+      </c>
+      <c r="G419">
+        <v>33.4</v>
+      </c>
+      <c r="H419">
+        <v>100</v>
+      </c>
+      <c r="I419">
+        <v>100</v>
+      </c>
+      <c r="T419">
+        <v>41.8</v>
+      </c>
+      <c r="U419">
+        <v>91</v>
+      </c>
+      <c r="V419">
+        <v>40.5</v>
+      </c>
+      <c r="W419">
+        <v>52</v>
+      </c>
+      <c r="X419">
+        <v>23.3</v>
+      </c>
+      <c r="Y419">
+        <v>29</v>
+      </c>
+      <c r="Z419">
+        <v>13.6</v>
+      </c>
+      <c r="AA419">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="420" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>49</v>
+      </c>
+      <c r="B420" t="s">
+        <v>33</v>
+      </c>
+      <c r="C420">
+        <v>25</v>
+      </c>
+      <c r="D420" t="s">
+        <v>30</v>
+      </c>
+      <c r="E420">
+        <v>100</v>
+      </c>
+      <c r="F420">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="G420">
+        <v>44.2</v>
+      </c>
+      <c r="H420">
+        <v>100</v>
+      </c>
+      <c r="I420">
+        <v>100</v>
+      </c>
+      <c r="T420">
+        <v>43.6</v>
+      </c>
+      <c r="U420">
+        <v>90</v>
+      </c>
+      <c r="V420">
+        <v>54.2</v>
+      </c>
+      <c r="W420">
+        <v>14</v>
+      </c>
+      <c r="X420">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="Y420">
+        <v>12</v>
+      </c>
+      <c r="Z420">
+        <v>25.2</v>
+      </c>
+      <c r="AA420">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="421" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>49</v>
+      </c>
+      <c r="B421" t="s">
+        <v>34</v>
+      </c>
+      <c r="C421">
+        <v>5</v>
+      </c>
+      <c r="D421" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="422" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>49</v>
+      </c>
+      <c r="B422" t="s">
+        <v>34</v>
+      </c>
+      <c r="C422">
+        <v>5</v>
+      </c>
+      <c r="D422" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="423" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>49</v>
+      </c>
+      <c r="B423" t="s">
+        <v>34</v>
+      </c>
+      <c r="C423">
+        <v>5</v>
+      </c>
+      <c r="D423" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="424" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>49</v>
+      </c>
+      <c r="B424" t="s">
+        <v>34</v>
+      </c>
+      <c r="C424">
+        <v>10</v>
+      </c>
+      <c r="D424" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="425" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>49</v>
+      </c>
+      <c r="B425" t="s">
+        <v>34</v>
+      </c>
+      <c r="C425">
+        <v>10</v>
+      </c>
+      <c r="D425" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="426" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>49</v>
+      </c>
+      <c r="B426" t="s">
+        <v>34</v>
+      </c>
+      <c r="C426">
+        <v>10</v>
+      </c>
+      <c r="D426" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="427" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>49</v>
+      </c>
+      <c r="B427" t="s">
+        <v>34</v>
+      </c>
+      <c r="C427">
+        <v>15</v>
+      </c>
+      <c r="D427" t="s">
+        <v>26</v>
+      </c>
+      <c r="E427">
+        <v>66.2</v>
+      </c>
+      <c r="F427">
+        <v>58.6</v>
+      </c>
+      <c r="G427">
+        <v>24.6</v>
+      </c>
+      <c r="H427">
+        <v>100</v>
+      </c>
+      <c r="I427">
+        <v>42.8</v>
+      </c>
+      <c r="T427">
+        <v>43</v>
+      </c>
+      <c r="U427">
+        <v>99</v>
+      </c>
+      <c r="V427">
+        <v>42.5</v>
+      </c>
+      <c r="W427">
+        <v>41</v>
+      </c>
+      <c r="X427">
+        <v>45.3</v>
+      </c>
+      <c r="Y427">
+        <v>15</v>
+      </c>
+      <c r="Z427">
+        <v>29.3</v>
+      </c>
+      <c r="AA427">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="428" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>49</v>
+      </c>
+      <c r="B428" t="s">
+        <v>34</v>
+      </c>
+      <c r="C428">
+        <v>15</v>
+      </c>
+      <c r="D428" t="s">
+        <v>29</v>
+      </c>
+      <c r="E428">
+        <v>99.8</v>
+      </c>
+      <c r="F428">
+        <v>67</v>
+      </c>
+      <c r="G428">
+        <v>30.3</v>
+      </c>
+      <c r="H428">
+        <v>100</v>
+      </c>
+      <c r="I428">
+        <v>99.6</v>
+      </c>
+      <c r="T428">
+        <v>41.8</v>
+      </c>
+      <c r="U428">
+        <v>94</v>
+      </c>
+      <c r="V428">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="W428">
+        <v>40</v>
+      </c>
+      <c r="X428">
+        <v>30.3</v>
+      </c>
+      <c r="Y428">
+        <v>17</v>
+      </c>
+      <c r="Z428">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="AA428">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="429" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>49</v>
+      </c>
+      <c r="B429" t="s">
+        <v>34</v>
+      </c>
+      <c r="C429">
+        <v>15</v>
+      </c>
+      <c r="D429" t="s">
+        <v>30</v>
+      </c>
+      <c r="E429">
+        <v>96.9</v>
+      </c>
+      <c r="F429">
+        <v>62.9</v>
+      </c>
+      <c r="G429">
+        <v>18.7</v>
+      </c>
+      <c r="H429">
+        <v>100</v>
+      </c>
+      <c r="I429">
+        <v>95.4</v>
+      </c>
+      <c r="T429">
+        <v>43.1</v>
+      </c>
+      <c r="U429">
+        <v>100</v>
+      </c>
+      <c r="V429">
+        <v>48.6</v>
+      </c>
+      <c r="W429">
+        <v>23</v>
+      </c>
+      <c r="X429">
+        <v>31.9</v>
+      </c>
+      <c r="Y429">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="430" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>49</v>
+      </c>
+      <c r="B430" t="s">
+        <v>34</v>
+      </c>
+      <c r="C430">
+        <v>20</v>
+      </c>
+      <c r="D430" t="s">
+        <v>26</v>
+      </c>
+      <c r="E430">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="F430">
+        <v>60.4</v>
+      </c>
+      <c r="G430">
+        <v>36</v>
+      </c>
+      <c r="H430">
+        <v>100</v>
+      </c>
+      <c r="I430">
+        <v>51.7</v>
+      </c>
+      <c r="T430">
+        <v>43</v>
+      </c>
+      <c r="U430">
+        <v>100</v>
+      </c>
+      <c r="V430">
+        <v>42.1</v>
+      </c>
+      <c r="W430">
+        <v>40</v>
+      </c>
+      <c r="X430">
+        <v>43.7</v>
+      </c>
+      <c r="Y430">
+        <v>11</v>
+      </c>
+      <c r="Z430">
+        <v>37.6</v>
+      </c>
+      <c r="AA430">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="431" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>49</v>
+      </c>
+      <c r="B431" t="s">
+        <v>34</v>
+      </c>
+      <c r="C431">
+        <v>20</v>
+      </c>
+      <c r="D431" t="s">
+        <v>29</v>
+      </c>
+      <c r="E431">
+        <v>100</v>
+      </c>
+      <c r="F431">
+        <v>68</v>
+      </c>
+      <c r="G431">
+        <v>31.9</v>
+      </c>
+      <c r="H431">
+        <v>100</v>
+      </c>
+      <c r="I431">
+        <v>99.9</v>
+      </c>
+      <c r="T431">
+        <v>42.2</v>
+      </c>
+      <c r="U431">
+        <v>91</v>
+      </c>
+      <c r="V431">
+        <v>39.299999999999997</v>
+      </c>
+      <c r="W431">
+        <v>45</v>
+      </c>
+      <c r="X431">
+        <v>26.3</v>
+      </c>
+      <c r="Y431">
+        <v>19</v>
+      </c>
+      <c r="Z431">
+        <v>15.4</v>
+      </c>
+      <c r="AA431">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="432" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>49</v>
+      </c>
+      <c r="B432" t="s">
+        <v>34</v>
+      </c>
+      <c r="C432">
+        <v>20</v>
+      </c>
+      <c r="D432" t="s">
+        <v>30</v>
+      </c>
+      <c r="E432">
+        <v>99.8</v>
+      </c>
+      <c r="F432">
+        <v>69.2</v>
+      </c>
+      <c r="G432">
+        <v>30.2</v>
+      </c>
+      <c r="H432">
+        <v>100</v>
+      </c>
+      <c r="I432">
+        <v>99.8</v>
+      </c>
+      <c r="T432">
+        <v>43</v>
+      </c>
+      <c r="U432">
+        <v>100</v>
+      </c>
+      <c r="V432">
+        <v>48.5</v>
+      </c>
+      <c r="W432">
+        <v>11</v>
+      </c>
+      <c r="X432">
+        <v>29</v>
+      </c>
+      <c r="Y432">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="433" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>49</v>
+      </c>
+      <c r="B433" t="s">
+        <v>34</v>
+      </c>
+      <c r="C433">
+        <v>25</v>
+      </c>
+      <c r="D433" t="s">
+        <v>26</v>
+      </c>
+      <c r="E433">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="F433">
+        <v>60.1</v>
+      </c>
+      <c r="G433">
+        <v>37.5</v>
+      </c>
+      <c r="H433">
+        <v>100</v>
+      </c>
+      <c r="I433">
+        <v>57.2</v>
+      </c>
+      <c r="T433">
+        <v>43</v>
+      </c>
+      <c r="U433">
+        <v>100</v>
+      </c>
+      <c r="V433">
+        <v>40.4</v>
+      </c>
+      <c r="W433">
+        <v>24</v>
+      </c>
+      <c r="X433">
+        <v>40.1</v>
+      </c>
+      <c r="Y433">
+        <v>15</v>
+      </c>
+      <c r="Z433">
+        <v>37.5</v>
+      </c>
+      <c r="AA433">
+        <v>15</v>
+      </c>
+      <c r="AB433">
+        <v>34.6</v>
+      </c>
+      <c r="AC433">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="434" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>49</v>
+      </c>
+      <c r="B434" t="s">
+        <v>34</v>
+      </c>
+      <c r="C434">
+        <v>25</v>
+      </c>
+      <c r="D434" t="s">
+        <v>29</v>
+      </c>
+      <c r="E434">
+        <v>100</v>
+      </c>
+      <c r="F434">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="G434">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="H434">
+        <v>100</v>
+      </c>
+      <c r="I434">
+        <v>100</v>
+      </c>
+      <c r="T434">
+        <v>41.8</v>
+      </c>
+      <c r="U434">
+        <v>90</v>
+      </c>
+      <c r="V434">
+        <v>39.1</v>
+      </c>
+      <c r="W434">
+        <v>47</v>
+      </c>
+      <c r="X434">
+        <v>26.1</v>
+      </c>
+      <c r="Y434">
+        <v>21</v>
+      </c>
+      <c r="Z434">
+        <v>13.4</v>
+      </c>
+      <c r="AA434">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="435" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>49</v>
+      </c>
+      <c r="B435" t="s">
+        <v>34</v>
+      </c>
+      <c r="C435">
+        <v>25</v>
+      </c>
+      <c r="D435" t="s">
+        <v>30</v>
+      </c>
+      <c r="E435">
+        <v>100</v>
+      </c>
+      <c r="F435">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="G435">
+        <v>32.4</v>
+      </c>
+      <c r="H435">
+        <v>100</v>
+      </c>
+      <c r="I435">
+        <v>100</v>
+      </c>
+      <c r="T435">
+        <v>43.2</v>
+      </c>
+      <c r="U435">
+        <v>98</v>
+      </c>
+      <c r="V435">
+        <v>47.3</v>
+      </c>
+      <c r="W435">
+        <v>14</v>
+      </c>
+      <c r="X435">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="Y435">
+        <v>10</v>
+      </c>
+      <c r="Z435">
+        <v>19.3</v>
+      </c>
+      <c r="AA435">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="436" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>50</v>
+      </c>
+      <c r="B436" t="s">
+        <v>34</v>
+      </c>
+      <c r="C436">
+        <v>15</v>
+      </c>
+      <c r="D436" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AC343" xr:uid="{3CACE78E-09B0-4A51-A9AF-2F3B2E4BAEFC}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC343">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AC390">
       <sortCondition ref="A2:A97"/>
       <sortCondition ref="B2:B97"/>
       <sortCondition ref="C2:C97"/>

</xml_diff>